<commit_message>
update and add data ++ add eventListerner ++ add ;> , csv explanation
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="177">
   <si>
     <t xml:space="preserve">27.0 </t>
   </si>
@@ -538,6 +538,18 @@
   </si>
   <si>
     <t>bpm-per-inwoner</t>
+  </si>
+  <si>
+    <t>absoluut-inwoner-aantal</t>
+  </si>
+  <si>
+    <t>absoluut-vluchtelingen-2015</t>
+  </si>
+  <si>
+    <t>minimumloon-mnd</t>
+  </si>
+  <si>
+    <t>vluchteling-10k-inwoner</t>
   </si>
 </sst>
 </file>
@@ -547,7 +559,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -572,15 +584,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -600,7 +615,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="275">
+  <cellStyleXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -876,19 +891,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="275">
+  <cellStyles count="293">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1026,6 +1067,15 @@
     <cellStyle name="Gevolgde hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1163,6 +1213,15 @@
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1492,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1505,55 +1564,71 @@
     <col min="4" max="4" width="5.375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.625" style="1"/>
+    <col min="7" max="10" width="10.625" style="1"/>
+    <col min="11" max="11" width="10.625" style="10"/>
+    <col min="12" max="12" width="10.625" style="12"/>
+    <col min="13" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>102.9</v>
       </c>
       <c r="G2" s="3">
@@ -1562,27 +1637,40 @@
       <c r="H2" s="3">
         <v>5.4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
+      <c r="J2" s="14">
+        <v>41300</v>
+      </c>
+      <c r="K2" s="5">
+        <v>8584926</v>
+      </c>
+      <c r="L2" s="5">
+        <f>SUM(J2/K2*10000)</f>
+        <v>48.107578329737493</v>
+      </c>
+      <c r="M2" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="4">
         <v>368.8</v>
       </c>
       <c r="G3" s="3">
@@ -1591,27 +1679,40 @@
       <c r="H3" s="3">
         <v>7.9</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
+      <c r="J3" s="14">
+        <v>17490</v>
+      </c>
+      <c r="K3" s="5">
+        <v>11258434</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" ref="L3:L36" si="0">SUM(J3/K3*10000)</f>
+        <v>15.535020234608117</v>
+      </c>
+      <c r="M3" s="13">
+        <v>1501.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>66.7</v>
       </c>
       <c r="G4" s="3">
@@ -1620,56 +1721,82 @@
       <c r="H4" s="3">
         <v>10.4</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="1">
-        <v>202.3</v>
+      <c r="J4" s="14">
+        <v>10700</v>
+      </c>
+      <c r="K4" s="5">
+        <v>7202198</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" si="0"/>
+        <v>14.856575728687272</v>
+      </c>
+      <c r="M4" s="13">
+        <v>194.29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="4">
+        <v>75.2</v>
       </c>
       <c r="G5" s="3">
-        <v>-1</v>
+        <v>16.5</v>
       </c>
       <c r="H5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I5">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
+        <v>18.3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>59</v>
+      </c>
+      <c r="J5" s="14">
+        <v>135</v>
+      </c>
+      <c r="K5" s="5">
+        <v>4225316</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31950273068333823</v>
+      </c>
+      <c r="M5" s="13">
+        <v>398.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>93.5</v>
       </c>
       <c r="G6" s="3">
@@ -1678,27 +1805,40 @@
       <c r="H6" s="3">
         <v>15.1</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
+      <c r="J6" s="14">
+        <v>1225</v>
+      </c>
+      <c r="K6" s="5">
+        <v>847008</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" si="0"/>
+        <v>14.462673315954511</v>
+      </c>
+      <c r="M6" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>136.1</v>
       </c>
       <c r="G7" s="3">
@@ -1707,839 +1847,1213 @@
       <c r="H7" s="3">
         <v>7.4</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="1">
-        <v>230</v>
+      <c r="J7" s="14">
+        <v>1010</v>
+      </c>
+      <c r="K7" s="5">
+        <v>10538275</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.95841112516042715</v>
+      </c>
+      <c r="M7" s="13">
+        <v>337.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="4">
+        <v>130.80000000000001</v>
       </c>
       <c r="G8" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
       <c r="H8" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="I8">
+        <v>6.8</v>
+      </c>
+      <c r="I8" s="4">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="1">
-        <v>130.80000000000001</v>
+      <c r="J8" s="14">
+        <v>5865</v>
+      </c>
+      <c r="K8" s="5">
+        <v>5659715</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" si="0"/>
+        <v>10.362712610087257</v>
+      </c>
+      <c r="M8" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="4">
+        <v>30.3</v>
       </c>
       <c r="G9" s="3">
-        <v>6.4</v>
+        <v>7.9</v>
       </c>
       <c r="H9" s="3">
         <v>6.8</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
+        <v>73</v>
+      </c>
+      <c r="J9" s="14">
+        <v>145</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1313271</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1041133170533728</v>
+      </c>
+      <c r="M9" s="13">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G10" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="4">
+        <v>110</v>
+      </c>
+      <c r="J10" s="14">
+        <v>4495</v>
+      </c>
+      <c r="K10" s="5">
+        <v>5471753</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" si="0"/>
+        <v>8.2149175958783225</v>
+      </c>
+      <c r="M10" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="4">
+        <v>103.8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4">
+        <v>107</v>
+      </c>
+      <c r="J11" s="14">
+        <v>43725</v>
+      </c>
+      <c r="K11" s="5">
+        <v>66352469</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5898075322562608</v>
+      </c>
+      <c r="M11" s="13">
+        <v>1457.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="4">
+        <v>230</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I12" s="4">
         <v>124</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="J12" s="14">
+        <v>229630</v>
+      </c>
+      <c r="K12" s="5">
+        <v>81174000</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="0"/>
+        <v>28.288614581023481</v>
+      </c>
+      <c r="M12" s="13">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4">
+        <v>84</v>
+      </c>
+      <c r="G13" s="3">
+        <v>23.7</v>
+      </c>
+      <c r="H13" s="3">
+        <v>30.2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>72</v>
+      </c>
+      <c r="J13" s="14">
+        <v>8430</v>
+      </c>
+      <c r="K13" s="5">
+        <v>10812467</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="0"/>
+        <v>7.7965555871754333</v>
+      </c>
+      <c r="M13" s="13">
+        <v>683.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="4">
+        <v>106.4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="H14" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="I14" s="4">
+        <v>68</v>
+      </c>
+      <c r="J14" s="14">
+        <v>112145</v>
+      </c>
+      <c r="K14" s="5">
+        <v>9849000</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="0"/>
+        <v>113.86435171083357</v>
+      </c>
+      <c r="M14" s="13">
+        <v>333.41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I15" s="4">
+        <v>121</v>
+      </c>
+      <c r="J15" s="14">
+        <v>135</v>
+      </c>
+      <c r="K15" s="5">
+        <v>329100</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="0"/>
+        <v>4.102096627164995</v>
+      </c>
+      <c r="M15" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="4">
+        <v>67.2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>12.9</v>
+      </c>
+      <c r="H16" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="I16" s="7">
+        <v>132</v>
+      </c>
+      <c r="J16" s="14">
+        <v>1940</v>
+      </c>
+      <c r="K16" s="5">
+        <v>4625885</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" si="0"/>
+        <v>4.1937921068076705</v>
+      </c>
+      <c r="M16" s="13">
+        <v>1461.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="4">
+        <v>199.4</v>
+      </c>
+      <c r="G17" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="H17" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="I17" s="4">
+        <v>97</v>
+      </c>
+      <c r="J17" s="14">
+        <v>44805</v>
+      </c>
+      <c r="K17" s="5">
+        <v>60795612</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="0"/>
+        <v>7.3697753054940875</v>
+      </c>
+      <c r="M17" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="4">
+        <v>32.4</v>
+      </c>
+      <c r="G18" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="H18" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I18" s="4">
+        <v>64</v>
+      </c>
+      <c r="J18" s="14">
+        <v>215</v>
+      </c>
+      <c r="K18" s="5">
+        <v>1986096</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0825257187970772</v>
+      </c>
+      <c r="M18" s="13">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="4">
+        <v>236.8</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I19" s="6">
+        <v>-1</v>
+      </c>
+      <c r="J19" s="14">
+        <v>75</v>
+      </c>
+      <c r="K19" s="5">
+        <v>37369</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="0"/>
+        <v>20.070111589820442</v>
+      </c>
+      <c r="M19" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="4">
+        <v>47.2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I20" s="4">
+        <v>74</v>
+      </c>
+      <c r="J20" s="14">
+        <v>245</v>
+      </c>
+      <c r="K20" s="5">
+        <v>2921262</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.83867862588155395</v>
+      </c>
+      <c r="M20" s="13">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="4">
+        <v>210.1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="H21" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="I21" s="4">
+        <v>263</v>
+      </c>
+      <c r="J21" s="14">
+        <v>770</v>
+      </c>
+      <c r="K21" s="5">
+        <v>562958</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" si="0"/>
+        <v>13.677752159130877</v>
+      </c>
+      <c r="M21" s="13">
+        <v>1922.96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1339.8</v>
+      </c>
+      <c r="G22" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="I22" s="4">
+        <v>85</v>
+      </c>
+      <c r="J22" s="14">
+        <v>1075</v>
+      </c>
+      <c r="K22" s="5">
+        <v>429344</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="0"/>
+        <v>25.038197808750091</v>
+      </c>
+      <c r="M22" s="13">
+        <v>720.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="4">
+        <v>45</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>39</v>
+      </c>
+      <c r="J23" s="14">
+        <v>-1</v>
+      </c>
+      <c r="K23" s="5">
+        <v>622099</v>
+      </c>
+      <c r="L23" s="5">
+        <v>-1</v>
+      </c>
+      <c r="M23" s="13">
+        <v>288.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="4">
+        <v>498.4</v>
+      </c>
+      <c r="G24" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="H24" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="I24" s="4">
+        <v>130</v>
+      </c>
+      <c r="J24" s="14">
+        <v>14350</v>
+      </c>
+      <c r="K24" s="5">
+        <v>16900726</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" si="0"/>
+        <v>8.4907595093843895</v>
+      </c>
+      <c r="M24" s="13">
+        <v>1507.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="4">
+        <v>16.7</v>
+      </c>
+      <c r="G25" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="I25" s="4">
+        <v>179</v>
+      </c>
+      <c r="J25" s="14">
+        <v>6775</v>
+      </c>
+      <c r="K25" s="5">
+        <v>5165802</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" si="0"/>
+        <v>13.115098100933794</v>
+      </c>
+      <c r="M25" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="4">
+        <v>121.7</v>
+      </c>
+      <c r="G26" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="I26" s="4">
+        <v>68</v>
+      </c>
+      <c r="J26" s="14">
+        <v>5920</v>
+      </c>
+      <c r="K26" s="5">
+        <v>38005614</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5576646123912115</v>
+      </c>
+      <c r="M26" s="13">
+        <v>417.55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="4">
+        <v>113.4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>7.3</v>
+      </c>
+      <c r="H27" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="I27" s="4">
+        <v>78</v>
+      </c>
+      <c r="J27" s="14">
+        <v>540</v>
+      </c>
+      <c r="K27" s="5">
+        <v>10374822</v>
+      </c>
+      <c r="L27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.52049085757808666</v>
+      </c>
+      <c r="M27" s="13">
+        <v>589.16999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="4">
+        <v>86.9</v>
+      </c>
+      <c r="G28" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I28" s="4">
+        <v>54</v>
+      </c>
+      <c r="J28" s="14">
+        <v>925</v>
+      </c>
+      <c r="K28" s="5">
+        <v>19861408</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.46572730392528061</v>
+      </c>
+      <c r="M28" s="13">
+        <v>234.77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="8">
+        <v>-1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="H29" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="I29" s="4">
+        <v>35</v>
+      </c>
+      <c r="J29" s="14">
+        <v>-1</v>
+      </c>
+      <c r="K29" s="5">
+        <v>-1</v>
+      </c>
+      <c r="L29" s="5">
+        <v>-1</v>
+      </c>
+      <c r="M29" s="13">
+        <v>235.51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="4">
+        <v>110.4</v>
+      </c>
+      <c r="G30" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="H30" s="3">
+        <v>13.6</v>
+      </c>
+      <c r="I30" s="4">
+        <v>83</v>
+      </c>
+      <c r="J30" s="14">
+        <v>160</v>
+      </c>
+      <c r="K30" s="5">
+        <v>5421349</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.29512949636704816</v>
+      </c>
+      <c r="M30" s="13">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="4">
+        <v>102.3</v>
+      </c>
+      <c r="G31" s="3">
+        <v>9</v>
+      </c>
+      <c r="H31" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="I31" s="4">
+        <v>76</v>
+      </c>
+      <c r="J31" s="14">
         <v>150</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="1">
-        <v>30.3</v>
-      </c>
-      <c r="G10" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="H10" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="I10">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
+      <c r="K31" s="5">
+        <v>2062874</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.72714087239453296</v>
+      </c>
+      <c r="M31" s="13">
+        <v>790.73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F32" s="4">
         <v>92.9</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G32" s="3">
         <v>23.6</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H32" s="3">
         <v>25.4</v>
       </c>
-      <c r="I11">
+      <c r="I32" s="4">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="1">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="G12" s="3">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="H12" s="3">
-        <v>8</v>
-      </c>
-      <c r="I12">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="1">
-        <v>103.8</v>
-      </c>
-      <c r="G13" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="H13" s="3">
-        <v>10</v>
-      </c>
-      <c r="I13">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="1">
-        <v>75.2</v>
-      </c>
-      <c r="G14" s="3">
-        <v>16.5</v>
-      </c>
-      <c r="H14" s="3">
-        <v>18.3</v>
-      </c>
-      <c r="I14">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="1">
-        <v>106.4</v>
-      </c>
-      <c r="G15" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="H15" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="I15">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="1">
-        <v>84</v>
-      </c>
-      <c r="G16" s="3">
-        <v>23.7</v>
-      </c>
-      <c r="H16" s="3">
-        <v>30.2</v>
-      </c>
-      <c r="I16">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="1">
-        <v>67.2</v>
-      </c>
-      <c r="G17" s="3">
-        <v>12.9</v>
-      </c>
-      <c r="H17" s="3">
-        <v>9.4</v>
-      </c>
-      <c r="I17" s="6">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="G18" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H18" s="3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="I18">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="1">
-        <v>199.4</v>
-      </c>
-      <c r="G19" s="3">
-        <v>11.9</v>
-      </c>
-      <c r="H19" s="3">
-        <v>13.8</v>
-      </c>
-      <c r="I19">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="1">
-        <v>236.8</v>
-      </c>
-      <c r="G20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I20" s="5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="1">
-        <v>47.2</v>
-      </c>
-      <c r="G21" s="3">
-        <v>12.2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="I21">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="1">
-        <v>210.1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="H22" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="I22">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2" t="s">
+      <c r="J32" s="14">
+        <v>7265</v>
+      </c>
+      <c r="K32" s="5">
+        <v>46439864</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5643887329213539</v>
+      </c>
+      <c r="M32" s="13">
+        <v>756.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="G33" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H33" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="I33" s="4">
+        <v>124</v>
+      </c>
+      <c r="J33" s="14">
+        <v>43945</v>
+      </c>
+      <c r="K33" s="5">
+        <v>9747355</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="0"/>
+        <v>45.084025358674225</v>
+      </c>
+      <c r="M33" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="4">
+        <v>202.3</v>
+      </c>
+      <c r="G34" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I34" s="4">
+        <v>161</v>
+      </c>
+      <c r="J34" s="14">
+        <v>17240</v>
+      </c>
+      <c r="K34" s="5">
+        <v>8236573</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" si="0"/>
+        <v>20.931035274015056</v>
+      </c>
+      <c r="M34" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="4">
+        <v>98.9</v>
+      </c>
+      <c r="G35" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I35" s="4">
         <v>53</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="1">
-        <v>32.4</v>
-      </c>
-      <c r="G23" s="3">
-        <v>11.8</v>
-      </c>
-      <c r="H23" s="3">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="I23">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="1">
-        <v>45</v>
-      </c>
-      <c r="G24" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H24" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I24">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1339.8</v>
-      </c>
-      <c r="G25" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="H25" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="I25">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="1">
-        <v>498.4</v>
-      </c>
-      <c r="G26" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="H26" s="3">
-        <v>7.8</v>
-      </c>
-      <c r="I26">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="1">
-        <v>16.7</v>
-      </c>
-      <c r="G27" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3.3</v>
-      </c>
-      <c r="I27">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="1">
-        <v>121.7</v>
-      </c>
-      <c r="G28" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="H28" s="3">
-        <v>9.6</v>
-      </c>
-      <c r="I28">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="1">
-        <v>113.4</v>
-      </c>
-      <c r="G29" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="H29" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="I29">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" s="1">
-        <v>86.9</v>
-      </c>
-      <c r="G30" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H30" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I30">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G31" s="3">
-        <v>13.8</v>
-      </c>
-      <c r="H31" s="3">
-        <v>14.5</v>
-      </c>
-      <c r="I31">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F32" s="1">
-        <v>23.6</v>
-      </c>
-      <c r="G32" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H32" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="I32">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="1">
-        <v>102.3</v>
-      </c>
-      <c r="G33" s="3">
-        <v>9</v>
-      </c>
-      <c r="H33" s="3">
-        <v>10.6</v>
-      </c>
-      <c r="I33">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="1">
-        <v>110.4</v>
-      </c>
-      <c r="G34" s="3">
-        <v>12.8</v>
-      </c>
-      <c r="H34" s="3">
-        <v>13.6</v>
-      </c>
-      <c r="I34">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" s="1">
-        <v>98.9</v>
-      </c>
-      <c r="G35" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H35" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I35">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="2" t="s">
+      <c r="J35" s="14">
+        <v>-1</v>
+      </c>
+      <c r="K35" s="5">
+        <v>77695904</v>
+      </c>
+      <c r="L35" s="5">
+        <v>-1</v>
+      </c>
+      <c r="M35" s="13">
+        <v>425.17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="4">
         <v>264.3</v>
       </c>
       <c r="G36" s="3">
@@ -2548,8 +3062,21 @@
       <c r="H36" s="3">
         <v>5.8</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="4">
         <v>108</v>
+      </c>
+      <c r="J36" s="14">
+        <v>21845</v>
+      </c>
+      <c r="K36" s="5">
+        <v>64767115</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" si="0"/>
+        <v>3.372853646484022</v>
+      </c>
+      <c r="M36" s="13">
+        <v>1509.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add offline jquery,map box,css code ++ add content data,json,csv ++ add icons
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="180">
   <si>
     <t xml:space="preserve">27.0 </t>
   </si>
@@ -549,7 +549,16 @@
     <t>minimumloon-mnd</t>
   </si>
   <si>
+    <t>absoluut-gino</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
     <t>vluchteling-10k-inwoner</t>
+  </si>
+  <si>
+    <t>uurloon-gemiddelde</t>
   </si>
 </sst>
 </file>
@@ -559,7 +568,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -597,6 +606,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -615,7 +631,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="293">
+  <cellStyleXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -909,8 +925,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -928,8 +970,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="293">
+  <cellStyles count="319">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1076,6 +1119,19 @@
     <cellStyle name="Gevolgde hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1222,6 +1278,19 @@
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1551,26 +1620,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="24.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.625" style="1"/>
-    <col min="11" max="11" width="10.625" style="10"/>
-    <col min="12" max="12" width="10.625" style="12"/>
-    <col min="13" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.75" style="10" customWidth="1"/>
+    <col min="13" max="13" width="4.125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="4.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4.25" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="4" t="s">
         <v>101</v>
       </c>
@@ -1580,39 +1656,44 @@
       <c r="C1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -1622,39 +1703,46 @@
       <c r="C2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="5">
+        <f>(31-E2)</f>
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>102.9</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>5.9</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>5.4</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>128</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="14">
         <v>41300</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>8584926</v>
       </c>
-      <c r="L2" s="5">
-        <f>SUM(J2/K2*10000)</f>
+      <c r="M2" s="5">
+        <f>SUM(K2/L2*10000)</f>
         <v>48.107578329737493</v>
       </c>
-      <c r="M2" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="3">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
@@ -1664,39 +1752,46 @@
       <c r="C3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="5">
+        <f>(31-E3)</f>
+        <v>5.1000000000000014</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>368.8</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>9</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>7.9</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>119</v>
       </c>
-      <c r="J3" s="14">
+      <c r="K3" s="14">
         <v>17490</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
         <v>11258434</v>
       </c>
-      <c r="L3" s="5">
-        <f t="shared" ref="L3:L36" si="0">SUM(J3/K3*10000)</f>
+      <c r="M3" s="5">
+        <f>SUM(K3/L3*10000)</f>
         <v>15.535020234608117</v>
       </c>
-      <c r="M3" s="13">
+      <c r="N3" s="13">
         <v>1501.82</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -1706,39 +1801,46 @@
       <c r="C4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="5">
+        <f>(31-E4)</f>
+        <v>-4.3999999999999986</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>66.7</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>12.3</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>10.4</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>45</v>
       </c>
-      <c r="J4" s="14">
+      <c r="K4" s="14">
         <v>10700</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>7202198</v>
       </c>
-      <c r="L4" s="5">
-        <f t="shared" si="0"/>
+      <c r="M4" s="5">
+        <f>SUM(K4/L4*10000)</f>
         <v>14.856575728687272</v>
       </c>
-      <c r="M4" s="13">
+      <c r="N4" s="13">
         <v>194.29</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="5" t="s">
         <v>46</v>
       </c>
@@ -1748,39 +1850,46 @@
       <c r="C5" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="5">
+        <f>(31-E5)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>75.2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>16.5</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>18.3</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>59</v>
       </c>
-      <c r="J5" s="14">
+      <c r="K5" s="14">
         <v>135</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>4225316</v>
       </c>
-      <c r="L5" s="5">
-        <f t="shared" si="0"/>
+      <c r="M5" s="5">
+        <f>SUM(K5/L5*10000)</f>
         <v>0.31950273068333823</v>
       </c>
-      <c r="M5" s="13">
+      <c r="N5" s="13">
         <v>398.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="3">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
@@ -1790,39 +1899,46 @@
       <c r="C6" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="5">
+        <f>(31-E6)</f>
+        <v>-1.3999999999999986</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>93.5</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>17.100000000000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>15.1</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>85</v>
       </c>
-      <c r="J6" s="14">
+      <c r="K6" s="14">
         <v>1225</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>847008</v>
       </c>
-      <c r="L6" s="5">
-        <f t="shared" si="0"/>
+      <c r="M6" s="5">
+        <f>SUM(K6/L6*10000)</f>
         <v>14.462673315954511</v>
       </c>
-      <c r="M6" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O6" s="3">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1832,39 +1948,46 @@
       <c r="C7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="5">
+        <f>(31-E7)</f>
+        <v>6.3999999999999986</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>136.1</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>7.4</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>84</v>
       </c>
-      <c r="J7" s="14">
+      <c r="K7" s="14">
         <v>1010</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
         <v>10538275</v>
       </c>
-      <c r="L7" s="5">
-        <f t="shared" si="0"/>
+      <c r="M7" s="5">
+        <f>SUM(K7/L7*10000)</f>
         <v>0.95841112516042715</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>337.58</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="3">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -1874,39 +1997,46 @@
       <c r="C8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="5">
+        <f>(31-E8)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>130.80000000000001</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>6.4</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>6.8</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <v>124</v>
       </c>
-      <c r="J8" s="14">
+      <c r="K8" s="14">
         <v>5865</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>5659715</v>
       </c>
-      <c r="L8" s="5">
-        <f t="shared" si="0"/>
+      <c r="M8" s="5">
+        <f>SUM(K8/L8*10000)</f>
         <v>10.362712610087257</v>
       </c>
-      <c r="M8" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O8" s="3">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -1916,39 +2046,46 @@
       <c r="C9" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="5">
+        <f>(31-E9)</f>
+        <v>-1.8999999999999986</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>30.3</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>7.9</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>6.8</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>73</v>
       </c>
-      <c r="J9" s="14">
+      <c r="K9" s="14">
         <v>145</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="5">
         <v>1313271</v>
       </c>
-      <c r="L9" s="5">
-        <f t="shared" si="0"/>
+      <c r="M9" s="5">
+        <f>SUM(K9/L9*10000)</f>
         <v>1.1041133170533728</v>
       </c>
-      <c r="M9" s="13">
+      <c r="N9" s="13">
         <v>390</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -1958,39 +2095,46 @@
       <c r="C10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="5">
+        <f>(31-E10)</f>
+        <v>5.6000000000000014</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>17.899999999999999</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>8</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>110</v>
       </c>
-      <c r="J10" s="14">
+      <c r="K10" s="14">
         <v>4495</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="5">
         <v>5471753</v>
       </c>
-      <c r="L10" s="5">
-        <f t="shared" si="0"/>
+      <c r="M10" s="5">
+        <f>SUM(K10/L10*10000)</f>
         <v>8.2149175958783225</v>
       </c>
-      <c r="M10" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O10" s="3">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
@@ -2000,39 +2144,46 @@
       <c r="C11" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="5">
+        <f>(31-E11)</f>
+        <v>0.89999999999999858</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>103.8</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>10.5</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>10</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>107</v>
       </c>
-      <c r="J11" s="14">
+      <c r="K11" s="14">
         <v>43725</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>66352469</v>
       </c>
-      <c r="L11" s="5">
-        <f t="shared" si="0"/>
+      <c r="M11" s="5">
+        <f>SUM(K11/L11*10000)</f>
         <v>6.5898075322562608</v>
       </c>
-      <c r="M11" s="13">
+      <c r="N11" s="13">
         <v>1457.52</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="3">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
@@ -2042,39 +2193,46 @@
       <c r="C12" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="5">
+        <f>(31-E12)</f>
+        <v>1.3000000000000007</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>230</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>5.3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>124</v>
       </c>
-      <c r="J12" s="14">
+      <c r="K12" s="14">
         <v>229630</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>81174000</v>
       </c>
-      <c r="L12" s="5">
-        <f t="shared" si="0"/>
+      <c r="M12" s="5">
+        <f>SUM(K12/L12*10000)</f>
         <v>28.288614581023481</v>
       </c>
-      <c r="M12" s="13">
+      <c r="N12" s="13">
         <v>1473</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" s="3">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
         <v>137</v>
       </c>
@@ -2084,39 +2242,46 @@
       <c r="C13" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="5">
+        <f>(31-E13)</f>
+        <v>-3.3999999999999986</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>84</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>23.7</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>30.2</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <v>72</v>
       </c>
-      <c r="J13" s="14">
+      <c r="K13" s="14">
         <v>8430</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="5">
         <v>10812467</v>
       </c>
-      <c r="L13" s="5">
-        <f t="shared" si="0"/>
+      <c r="M13" s="5">
+        <f>SUM(K13/L13*10000)</f>
         <v>7.7965555871754333</v>
       </c>
-      <c r="M13" s="13">
+      <c r="N13" s="13">
         <v>683.76</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13" s="3">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -2126,39 +2291,46 @@
       <c r="C14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="5">
+        <f>(31-E14)</f>
+        <v>3</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>106.4</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>7.6</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>7.9</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <v>68</v>
       </c>
-      <c r="J14" s="14">
+      <c r="K14" s="14">
         <v>112145</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L14" s="5">
         <v>9849000</v>
       </c>
-      <c r="L14" s="5">
-        <f t="shared" si="0"/>
+      <c r="M14" s="5">
+        <f>SUM(K14/L14*10000)</f>
         <v>113.86435171083357</v>
       </c>
-      <c r="M14" s="13">
+      <c r="N14" s="13">
         <v>333.41</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14" s="3">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
@@ -2168,39 +2340,46 @@
       <c r="C15" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="5">
+        <f>(31-E15)</f>
+        <v>7</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>3.2</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <v>121</v>
       </c>
-      <c r="J15" s="14">
+      <c r="K15" s="14">
         <v>135</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>329100</v>
       </c>
-      <c r="L15" s="5">
-        <f t="shared" si="0"/>
+      <c r="M15" s="5">
+        <f>SUM(K15/L15*10000)</f>
         <v>4.102096627164995</v>
       </c>
-      <c r="M15" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="N15" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="5" t="s">
         <v>48</v>
       </c>
@@ -2210,39 +2389,46 @@
       <c r="C16" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="5">
+        <f>(31-E16)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>67.2</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>12.9</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>9.4</v>
       </c>
-      <c r="I16" s="7">
+      <c r="J16" s="7">
         <v>132</v>
       </c>
-      <c r="J16" s="14">
+      <c r="K16" s="14">
         <v>1940</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>4625885</v>
       </c>
-      <c r="L16" s="5">
-        <f t="shared" si="0"/>
+      <c r="M16" s="5">
+        <f>SUM(K16/L16*10000)</f>
         <v>4.1937921068076705</v>
       </c>
-      <c r="M16" s="13">
+      <c r="N16" s="13">
         <v>1461.85</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16" s="3">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -2252,39 +2438,46 @@
       <c r="C17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="5">
+        <f>(31-E17)</f>
+        <v>-1.5</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>199.4</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>11.9</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>13.8</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <v>97</v>
       </c>
-      <c r="J17" s="14">
+      <c r="K17" s="14">
         <v>44805</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>60795612</v>
       </c>
-      <c r="L17" s="5">
-        <f t="shared" si="0"/>
+      <c r="M17" s="5">
+        <f>SUM(K17/L17*10000)</f>
         <v>7.3697753054940875</v>
       </c>
-      <c r="M17" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O17" s="3">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -2294,39 +2487,46 @@
       <c r="C18" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="5">
+        <f>(31-E18)</f>
+        <v>-4.2000000000000028</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>32.4</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>11.8</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <v>64</v>
       </c>
-      <c r="J18" s="14">
+      <c r="K18" s="14">
         <v>215</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="5">
         <v>1986096</v>
       </c>
-      <c r="L18" s="5">
-        <f t="shared" si="0"/>
+      <c r="M18" s="5">
+        <f>SUM(K18/L18*10000)</f>
         <v>1.0825257187970772</v>
       </c>
-      <c r="M18" s="13">
+      <c r="N18" s="13">
         <v>360</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18" s="3">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="5" t="s">
         <v>67</v>
       </c>
@@ -2336,39 +2536,45 @@
       <c r="C19" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="5">
-        <v>-1</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>236.8</v>
       </c>
-      <c r="G19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I19" s="6">
-        <v>-1</v>
-      </c>
-      <c r="J19" s="14">
+      <c r="H19" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K19" s="14">
         <v>75</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="5">
         <v>37369</v>
       </c>
-      <c r="L19" s="5">
-        <f t="shared" si="0"/>
+      <c r="M19" s="5">
+        <f>SUM(K19/L19*10000)</f>
         <v>20.070111589820442</v>
       </c>
-      <c r="M19" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="5" t="s">
         <v>51</v>
       </c>
@@ -2378,39 +2584,46 @@
       <c r="C20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="5">
+        <f>(31-E20)</f>
+        <v>-3.6000000000000014</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>47.2</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>12.2</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>74</v>
       </c>
-      <c r="J20" s="14">
+      <c r="K20" s="14">
         <v>245</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="5">
         <v>2921262</v>
       </c>
-      <c r="L20" s="5">
-        <f t="shared" si="0"/>
+      <c r="M20" s="5">
+        <f>SUM(K20/L20*10000)</f>
         <v>0.83867862588155395</v>
       </c>
-      <c r="M20" s="13">
+      <c r="N20" s="13">
         <v>325</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="O20" s="3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -2420,39 +2633,46 @@
       <c r="C21" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="5">
+        <f>(31-E21)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>210.1</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>5.8</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>6.3</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>263</v>
       </c>
-      <c r="J21" s="14">
+      <c r="K21" s="14">
         <v>770</v>
       </c>
-      <c r="K21" s="5">
+      <c r="L21" s="5">
         <v>562958</v>
       </c>
-      <c r="L21" s="5">
-        <f t="shared" si="0"/>
+      <c r="M21" s="5">
+        <f>SUM(K21/L21*10000)</f>
         <v>13.677752159130877</v>
       </c>
-      <c r="M21" s="13">
+      <c r="N21" s="13">
         <v>1922.96</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="O21" s="3">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="5" t="s">
         <v>55</v>
       </c>
@@ -2462,39 +2682,46 @@
       <c r="C22" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="5">
+        <f>(31-E22)</f>
+        <v>3.1000000000000014</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
         <v>1339.8</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>6.1</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>5.4</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <v>85</v>
       </c>
-      <c r="J22" s="14">
+      <c r="K22" s="14">
         <v>1075</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="5">
         <v>429344</v>
       </c>
-      <c r="L22" s="5">
-        <f t="shared" si="0"/>
+      <c r="M22" s="5">
+        <f>SUM(K22/L22*10000)</f>
         <v>25.038197808750091</v>
       </c>
-      <c r="M22" s="13">
+      <c r="N22" s="13">
         <v>720.46</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="O22" s="3">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="5" t="s">
         <v>54</v>
       </c>
@@ -2504,38 +2731,45 @@
       <c r="C23" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="5">
+        <f>(31-E23)</f>
+        <v>-6</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>45</v>
       </c>
-      <c r="G23" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H23" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I23" s="4">
+      <c r="H23" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J23" s="4">
         <v>39</v>
       </c>
-      <c r="J23" s="14">
-        <v>-1</v>
-      </c>
-      <c r="K23" s="5">
+      <c r="K23" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="L23" s="5">
         <v>622099</v>
       </c>
-      <c r="L23" s="5">
-        <v>-1</v>
-      </c>
-      <c r="M23" s="13">
+      <c r="M23" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" s="13">
         <v>288.05</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="O23" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
@@ -2545,39 +2779,46 @@
       <c r="C24" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="5">
+        <f>(31-E24)</f>
+        <v>5.8999999999999986</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G24" s="4">
         <v>498.4</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>7.2</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>7.8</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <v>130</v>
       </c>
-      <c r="J24" s="14">
+      <c r="K24" s="14">
         <v>14350</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>16900726</v>
       </c>
-      <c r="L24" s="5">
-        <f t="shared" si="0"/>
+      <c r="M24" s="5">
+        <f>SUM(K24/L24*10000)</f>
         <v>8.4907595093843895</v>
       </c>
-      <c r="M24" s="13">
+      <c r="N24" s="13">
         <v>1507.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="O24" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="5" t="s">
         <v>57</v>
       </c>
@@ -2587,39 +2828,46 @@
       <c r="C25" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="5">
+        <f>(31-E25)</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G25" s="4">
         <v>16.7</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H25" s="3">
         <v>3.7</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <v>3.3</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>179</v>
       </c>
-      <c r="J25" s="14">
+      <c r="K25" s="14">
         <v>6775</v>
       </c>
-      <c r="K25" s="5">
+      <c r="L25" s="5">
         <v>5165802</v>
       </c>
-      <c r="L25" s="5">
-        <f t="shared" si="0"/>
+      <c r="M25" s="5">
+        <f>SUM(K25/L25*10000)</f>
         <v>13.115098100933794</v>
       </c>
-      <c r="M25" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O25" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -2629,39 +2877,46 @@
       <c r="C26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="5">
+        <f>(31-E26)</f>
+        <v>0.30000000000000071</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
         <v>121.7</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="3">
         <v>8.5</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <v>9.6</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <v>68</v>
       </c>
-      <c r="J26" s="14">
+      <c r="K26" s="14">
         <v>5920</v>
       </c>
-      <c r="K26" s="5">
+      <c r="L26" s="5">
         <v>38005614</v>
       </c>
-      <c r="L26" s="5">
-        <f t="shared" si="0"/>
+      <c r="M26" s="5">
+        <f>SUM(K26/L26*10000)</f>
         <v>1.5576646123912115</v>
       </c>
-      <c r="M26" s="13">
+      <c r="N26" s="13">
         <v>417.55</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="O26" s="3">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -2671,39 +2926,46 @@
       <c r="C27" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="5">
+        <f>(31-E27)</f>
+        <v>-3.2000000000000028</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>113.4</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="3">
         <v>7.3</v>
       </c>
-      <c r="H27" s="3">
+      <c r="I27" s="3">
         <v>6.1</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <v>78</v>
       </c>
-      <c r="J27" s="14">
+      <c r="K27" s="14">
         <v>540</v>
       </c>
-      <c r="K27" s="5">
+      <c r="L27" s="5">
         <v>10374822</v>
       </c>
-      <c r="L27" s="5">
-        <f t="shared" si="0"/>
+      <c r="M27" s="5">
+        <f>SUM(K27/L27*10000)</f>
         <v>0.52049085757808666</v>
       </c>
-      <c r="M27" s="13">
+      <c r="N27" s="13">
         <v>589.16999999999996</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="O27" s="3">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -2713,39 +2975,46 @@
       <c r="C28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="5">
+        <f>(31-E28)</f>
+        <v>-3</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
         <v>86.9</v>
       </c>
-      <c r="G28" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H28" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I28" s="4">
+      <c r="H28" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J28" s="4">
         <v>54</v>
       </c>
-      <c r="J28" s="14">
+      <c r="K28" s="14">
         <v>925</v>
       </c>
-      <c r="K28" s="5">
+      <c r="L28" s="5">
         <v>19861408</v>
       </c>
-      <c r="L28" s="5">
-        <f t="shared" si="0"/>
+      <c r="M28" s="5">
+        <f>SUM(K28/L28*10000)</f>
         <v>0.46572730392528061</v>
       </c>
-      <c r="M28" s="13">
+      <c r="N28" s="13">
         <v>234.77</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="O28" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
@@ -2755,38 +3024,45 @@
       <c r="C29" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="5">
+        <f>(31-E29)</f>
+        <v>-7</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="4">
-        <v>-1</v>
-      </c>
-      <c r="F29" s="8">
-        <v>-1</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="F29" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="3">
         <v>13.8</v>
       </c>
-      <c r="H29" s="3">
+      <c r="I29" s="3">
         <v>14.5</v>
       </c>
-      <c r="I29" s="4">
+      <c r="J29" s="4">
         <v>35</v>
       </c>
-      <c r="J29" s="14">
-        <v>-1</v>
-      </c>
-      <c r="K29" s="5">
-        <v>-1</v>
-      </c>
-      <c r="L29" s="5">
-        <v>-1</v>
-      </c>
-      <c r="M29" s="13">
+      <c r="K29" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="N29" s="13">
         <v>235.51</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="O29" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="5" t="s">
         <v>64</v>
       </c>
@@ -2796,39 +3072,46 @@
       <c r="C30" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="5">
+        <f>(31-E30)</f>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="4">
+      <c r="G30" s="4">
         <v>110.4</v>
       </c>
-      <c r="G30" s="3">
+      <c r="H30" s="3">
         <v>12.8</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="3">
         <v>13.6</v>
       </c>
-      <c r="I30" s="4">
+      <c r="J30" s="4">
         <v>83</v>
       </c>
-      <c r="J30" s="14">
+      <c r="K30" s="14">
         <v>160</v>
       </c>
-      <c r="K30" s="5">
+      <c r="L30" s="5">
         <v>5421349</v>
       </c>
-      <c r="L30" s="5">
-        <f t="shared" si="0"/>
+      <c r="M30" s="5">
+        <f>SUM(K30/L30*10000)</f>
         <v>0.29512949636704816</v>
       </c>
-      <c r="M30" s="13">
+      <c r="N30" s="13">
         <v>380</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="O30" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="5" t="s">
         <v>63</v>
       </c>
@@ -2838,39 +3121,46 @@
       <c r="C31" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="5">
+        <f>(31-E31)</f>
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="4">
+      <c r="G31" s="4">
         <v>102.3</v>
       </c>
-      <c r="G31" s="3">
+      <c r="H31" s="3">
         <v>9</v>
       </c>
-      <c r="H31" s="3">
+      <c r="I31" s="3">
         <v>10.6</v>
       </c>
-      <c r="I31" s="4">
+      <c r="J31" s="4">
         <v>76</v>
       </c>
-      <c r="J31" s="14">
+      <c r="K31" s="14">
         <v>150</v>
       </c>
-      <c r="K31" s="5">
+      <c r="L31" s="5">
         <v>2062874</v>
       </c>
-      <c r="L31" s="5">
-        <f t="shared" si="0"/>
+      <c r="M31" s="5">
+        <f>SUM(K31/L31*10000)</f>
         <v>0.72714087239453296</v>
       </c>
-      <c r="M31" s="13">
+      <c r="N31" s="13">
         <v>790.73</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="O31" s="3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="5" t="s">
         <v>43</v>
       </c>
@@ -2880,39 +3170,46 @@
       <c r="C32" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="5">
+        <f>(31-E32)</f>
+        <v>-2.7000000000000028</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="4">
+      <c r="G32" s="4">
         <v>92.9</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H32" s="3">
         <v>23.6</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="3">
         <v>25.4</v>
       </c>
-      <c r="I32" s="4">
+      <c r="J32" s="4">
         <v>93</v>
       </c>
-      <c r="J32" s="14">
+      <c r="K32" s="14">
         <v>7265</v>
       </c>
-      <c r="K32" s="5">
+      <c r="L32" s="5">
         <v>46439864</v>
       </c>
-      <c r="L32" s="5">
-        <f t="shared" si="0"/>
+      <c r="M32" s="5">
+        <f>SUM(K32/L32*10000)</f>
         <v>1.5643887329213539</v>
       </c>
-      <c r="M32" s="13">
+      <c r="N32" s="13">
         <v>756.7</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="O32" s="3">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="5" t="s">
         <v>62</v>
       </c>
@@ -2922,39 +3219,46 @@
       <c r="C33" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="5">
+        <f>(31-E33)</f>
+        <v>6.1000000000000014</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F33" s="4">
+      <c r="G33" s="4">
         <v>23.6</v>
       </c>
-      <c r="G33" s="3">
+      <c r="H33" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>7.7</v>
       </c>
-      <c r="I33" s="4">
+      <c r="J33" s="4">
         <v>124</v>
       </c>
-      <c r="J33" s="14">
+      <c r="K33" s="14">
         <v>43945</v>
       </c>
-      <c r="K33" s="5">
+      <c r="L33" s="5">
         <v>9747355</v>
       </c>
-      <c r="L33" s="5">
-        <f t="shared" si="0"/>
+      <c r="M33" s="5">
+        <f>SUM(K33/L33*10000)</f>
         <v>45.084025358674225</v>
       </c>
-      <c r="M33" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O33" s="3">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="5" t="s">
         <v>37</v>
       </c>
@@ -2964,39 +3268,46 @@
       <c r="C34" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="5">
+        <f>(31-E34)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F34" s="4">
+      <c r="G34" s="4">
         <v>202.3</v>
       </c>
-      <c r="G34" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H34" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I34" s="4">
+      <c r="H34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J34" s="4">
         <v>161</v>
       </c>
-      <c r="J34" s="14">
+      <c r="K34" s="14">
         <v>17240</v>
       </c>
-      <c r="K34" s="5">
+      <c r="L34" s="5">
         <v>8236573</v>
       </c>
-      <c r="L34" s="5">
-        <f t="shared" si="0"/>
+      <c r="M34" s="5">
+        <f>SUM(K34/L34*10000)</f>
         <v>20.931035274015056</v>
       </c>
-      <c r="M34" s="13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="5" t="s">
         <v>65</v>
       </c>
@@ -3006,38 +3317,44 @@
       <c r="C35" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="5">
-        <v>-1</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="D35" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="4">
+      <c r="G35" s="4">
         <v>98.9</v>
       </c>
-      <c r="G35" s="3">
-        <v>-1</v>
-      </c>
-      <c r="H35" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I35" s="4">
+      <c r="H35" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J35" s="4">
         <v>53</v>
       </c>
-      <c r="J35" s="14">
-        <v>-1</v>
-      </c>
-      <c r="K35" s="5">
+      <c r="K35" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="L35" s="5">
         <v>77695904</v>
       </c>
-      <c r="L35" s="5">
-        <v>-1</v>
-      </c>
-      <c r="M35" s="13">
+      <c r="M35" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="N35" s="13">
         <v>425.17</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="O35" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="5" t="s">
         <v>66</v>
       </c>
@@ -3047,36 +3364,43 @@
       <c r="C36" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="5">
+        <f>(31-E36)</f>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="4">
+      <c r="G36" s="4">
         <v>264.3</v>
       </c>
-      <c r="G36" s="3">
+      <c r="H36" s="3">
         <v>6.4</v>
       </c>
-      <c r="H36" s="3">
+      <c r="I36" s="3">
         <v>5.8</v>
       </c>
-      <c r="I36" s="4">
+      <c r="J36" s="4">
         <v>108</v>
       </c>
-      <c r="J36" s="14">
+      <c r="K36" s="14">
         <v>21845</v>
       </c>
-      <c r="K36" s="5">
+      <c r="L36" s="5">
         <v>64767115</v>
       </c>
-      <c r="L36" s="5">
-        <f t="shared" si="0"/>
+      <c r="M36" s="5">
+        <f>SUM(K36/L36*10000)</f>
         <v>3.372853646484022</v>
       </c>
-      <c r="M36" s="13">
+      <c r="N36" s="13">
         <v>1509.7</v>
+      </c>
+      <c r="O36" s="3">
+        <v>22.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new feature fist one = blue++ update data => ,jobs-avail,werkloosheid, ++ add images
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -18,8 +18,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stefan</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Kans op een baan / hoeveelheid banen</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="189">
   <si>
     <t>AT</t>
   </si>
@@ -529,13 +563,70 @@
   </si>
   <si>
     <t>ME</t>
+  </si>
+  <si>
+    <t>jobs-avail</t>
+  </si>
+  <si>
+    <t>werkloosheid</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>2.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -577,6 +668,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -929,7 +1033,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -943,6 +1046,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="319">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1591,11 +1695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J36" sqref="A1:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1623,24 +1727,28 @@
       <c r="C1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="10"/>
+      <c r="I1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
@@ -1652,10 +1760,10 @@
       <c r="C2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>138</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1666,6 +1774,13 @@
       </c>
       <c r="H2" s="2">
         <v>2165</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="15">
+        <f>0.049*(0.845*G2)</f>
+        <v>355458.86103000003</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1678,10 +1793,10 @@
       <c r="C3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>137</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1690,10 +1805,16 @@
       <c r="G3" s="3">
         <v>11258434</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>2092</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="I3" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" s="15">
+        <f>0.073*(0.845*G3)</f>
+        <v>694476.50129000004</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
@@ -1705,10 +1826,10 @@
       <c r="C4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>14</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>139</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1719,6 +1840,13 @@
       </c>
       <c r="H4" s="2">
         <v>324</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="15">
+        <f>0.17*(0.845*G4)</f>
+        <v>1034595.7427000001</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1731,10 +1859,10 @@
       <c r="C5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>14</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>139</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1743,8 +1871,15 @@
       <c r="G5" s="3">
         <v>4225316</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>755</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="J5" s="15">
+        <f>0.146*(0.845*G5)</f>
+        <v>521277.23491999996</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1757,10 +1892,10 @@
       <c r="C6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>140</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1771,6 +1906,13 @@
       </c>
       <c r="H6" s="5">
         <v>2223</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="J6" s="15">
+        <f>0.14*(0.845*G6)</f>
+        <v>100201.04640000001</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1783,10 +1925,10 @@
       <c r="C7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>141</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1795,8 +1937,15 @@
       <c r="G7" s="3">
         <v>10538275</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>725</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="15">
+        <f>0.054*(0.845*G7)</f>
+        <v>480861.48824999999</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1809,10 +1958,10 @@
       <c r="C8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1821,8 +1970,15 @@
       <c r="G8" s="3">
         <v>5659715</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>2389</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" s="15">
+        <f>0.055*(0.845*G8)</f>
+        <v>263035.254625</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1835,10 +1991,10 @@
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>143</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1849,6 +2005,13 @@
       </c>
       <c r="H9" s="2">
         <v>832</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="J9" s="15">
+        <f>0.067*(0.845*G9)</f>
+        <v>74350.837664999999</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1861,10 +2024,10 @@
       <c r="C10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>144</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1875,6 +2038,13 @@
       </c>
       <c r="H10" s="2">
         <v>2479</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J10" s="15">
+        <f>0.07*(0.845*G10)</f>
+        <v>323654.18995000003</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1887,10 +2057,10 @@
       <c r="C11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>13</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>145</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1901,6 +2071,13 @@
       </c>
       <c r="H11" s="2">
         <v>2183</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J11" s="15">
+        <f>0.088*(0.845*G11)</f>
+        <v>4933969.5948399995</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1913,10 +2090,10 @@
       <c r="C12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>146</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1927,6 +2104,13 @@
       </c>
       <c r="H12" s="2">
         <v>2155</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J12" s="15">
+        <f>0.047*(0.845*G12)</f>
+        <v>3223825.41</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1939,10 +2123,10 @@
       <c r="C13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>147</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1951,8 +2135,15 @@
       <c r="G13" s="3">
         <v>10812467</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <v>1262</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13" s="15">
+        <f>0.248*(0.845*G13)</f>
+        <v>2265860.58452</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1965,10 +2156,10 @@
       <c r="C14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>8</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>148</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1977,8 +2168,15 @@
       <c r="G14" s="3">
         <v>9849000</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <v>532</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="J14" s="15">
+        <f>0.067*(0.845*G14)</f>
+        <v>557601.13500000001</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1991,10 +2189,10 @@
       <c r="C15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>6</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2003,8 +2201,15 @@
       <c r="G15" s="3">
         <v>329100</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="13">
         <v>2334</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J15" s="15">
+        <f>0.039*(0.845*G15)</f>
+        <v>10845.4905</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2017,10 +2222,10 @@
       <c r="C16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>13</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>145</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -2029,8 +2234,15 @@
       <c r="G16" s="3">
         <v>4625885</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <v>2186</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="J16" s="15">
+        <f>0.1*(0.845*G16)</f>
+        <v>390887.28249999997</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2043,10 +2255,10 @@
       <c r="C17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>149</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -2055,8 +2267,15 @@
       <c r="G17" s="3">
         <v>60795612</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <v>2030</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J17" s="15">
+        <f>0.16*(0.845*G17)</f>
+        <v>8219566.7423999999</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2069,10 +2288,10 @@
       <c r="C18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>16</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>36</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -2083,6 +2302,13 @@
       </c>
       <c r="H18" s="2">
         <v>379</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="J18" s="15">
+        <f>0.1*(0.845*G18)</f>
+        <v>167825.11199999999</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2095,10 +2321,10 @@
       <c r="C19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>158</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -2107,8 +2333,15 @@
       <c r="G19" s="3">
         <v>37369</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <v>5314</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" s="15">
+        <f>0.023*(0.845*G19)</f>
+        <v>726.26651500000003</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2121,10 +2354,10 @@
       <c r="C20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>140</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -2133,8 +2366,15 @@
       <c r="G20" s="3">
         <v>2921262</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>496</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="J20" s="15">
+        <f>0.099*(0.845*G20)</f>
+        <v>244378.17261000004</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2147,10 +2387,10 @@
       <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>150</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -2159,8 +2399,15 @@
       <c r="G21" s="3">
         <v>562958</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>3187</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="J21" s="15">
+        <f>0.05*(0.845*G21)</f>
+        <v>23784.9755</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2173,10 +2420,10 @@
       <c r="C22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <v>7</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -2185,8 +2432,15 @@
       <c r="G22" s="3">
         <v>429344</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="13">
         <v>1006</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" s="15">
+        <f>0.048*(0.845*G22)</f>
+        <v>17414.192640000001</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2199,10 +2453,10 @@
       <c r="C23" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>151</v>
       </c>
       <c r="F23" s="2" t="s">
@@ -2213,6 +2467,13 @@
       </c>
       <c r="H23" s="5">
         <v>726</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J23" s="15">
+        <f>0.145*(0.845*G23)</f>
+        <v>76222.679974999992</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2225,10 +2486,10 @@
       <c r="C24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <v>7</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>28</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -2237,8 +2498,15 @@
       <c r="G24" s="3">
         <v>16900726</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <v>2158</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="J24" s="15">
+        <f>0.065*(0.845*G24)</f>
+        <v>928272.37555</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2251,10 +2519,10 @@
       <c r="C25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>152</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -2265,6 +2533,13 @@
       </c>
       <c r="H25" s="5">
         <v>3850</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="J25" s="15">
+        <f>0.028*(0.845*G25)</f>
+        <v>122222.87531999999</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2277,10 +2552,10 @@
       <c r="C26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>153</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2291,6 +2566,13 @@
       </c>
       <c r="H26" s="5">
         <v>634</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J26" s="15">
+        <f>0.077*(0.845*G26)</f>
+        <v>2472835.2749099997</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2303,10 +2585,10 @@
       <c r="C27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="11">
         <v>16</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>154</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -2315,8 +2597,15 @@
       <c r="G27" s="3">
         <v>10374822</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <v>1056</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J27" s="15">
+        <f>0.125*(0.845*G27)</f>
+        <v>1095840.57375</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2329,10 +2618,10 @@
       <c r="C28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="11">
         <v>6</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>155</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -2341,10 +2630,16 @@
       <c r="G28" s="3">
         <v>19861408</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <v>345</v>
       </c>
-      <c r="J28"/>
+      <c r="I28" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="J28" s="15">
+        <f>0.055*(0.845*G28)</f>
+        <v>923058.93679999991</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
@@ -2356,10 +2651,10 @@
       <c r="C29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="11">
         <v>10</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>30</v>
       </c>
       <c r="F29" s="2">
@@ -2370,6 +2665,13 @@
       </c>
       <c r="H29" s="5">
         <v>377</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J29" s="15">
+        <f>0.2*(0.845*G29)</f>
+        <v>1183000</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2382,10 +2684,10 @@
       <c r="C30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>156</v>
       </c>
       <c r="F30" s="2" t="s">
@@ -2394,8 +2696,15 @@
       <c r="G30" s="3">
         <v>5421349</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <v>664</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="J30" s="15">
+        <f>0.118*(0.845*G30)</f>
+        <v>540562.70878999995</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2408,10 +2717,10 @@
       <c r="C31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="11">
         <v>5</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>157</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -2420,8 +2729,15 @@
       <c r="G31" s="3">
         <v>2062874</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="14">
         <v>1023</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="15">
+        <f>0.089*(0.845*G31)</f>
+        <v>155138.43917</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2434,10 +2750,10 @@
       <c r="C32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <v>16</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <v>36</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -2449,8 +2765,15 @@
       <c r="H32" s="5">
         <v>1702</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J32" s="15">
+        <f>0.223*(0.845*G32)</f>
+        <v>8750895.7728399988</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
@@ -2460,10 +2783,10 @@
       <c r="C33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="11">
         <v>6</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>155</v>
       </c>
       <c r="F33" s="2" t="s">
@@ -2475,8 +2798,15 @@
       <c r="H33" s="5">
         <v>2825</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="J33" s="15">
+        <f>0.057*(0.845*G33)</f>
+        <v>469481.35357500002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
@@ -2486,10 +2816,10 @@
       <c r="C34" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>158</v>
       </c>
       <c r="F34" s="2" t="s">
@@ -2501,8 +2831,15 @@
       <c r="H34" s="5">
         <v>2930</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="J34" s="15">
+        <f>0.034*(0.845*G34)</f>
+        <v>236636.74228999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
@@ -2512,10 +2849,10 @@
       <c r="C35" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="11">
         <v>20</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="10">
         <v>40</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -2524,11 +2861,18 @@
       <c r="G35" s="3">
         <v>77695904</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="14">
         <v>510</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J35" s="15">
+        <f>0.083*(0.845*G35)</f>
+        <v>5449202.2270400003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="3" t="s">
         <v>31</v>
       </c>
@@ -2538,10 +2882,10 @@
       <c r="C36" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="11">
         <v>10</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="10">
         <v>30.2</v>
       </c>
       <c r="F36" s="2" t="s">
@@ -2550,13 +2894,21 @@
       <c r="G36" s="3">
         <v>64767115</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="14">
         <v>2233</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="J36" s="15">
+        <f>0.044*(0.845*G36)</f>
+        <v>2408041.3356999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add discrimi data ++ add bestCountry sort feature variablesIsHighToLow ++ update data ++ add malta image
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="187">
   <si>
     <t>AT</t>
   </si>
@@ -160,9 +160,6 @@
     <t>12.8</t>
   </si>
   <si>
-    <t>31.42</t>
-  </si>
-  <si>
     <t>10.47</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>20.63</t>
   </si>
   <si>
-    <t>6.4</t>
-  </si>
-  <si>
     <t>21.89</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>11.39</t>
   </si>
   <si>
-    <t>45.87</t>
-  </si>
-  <si>
     <t>19.93</t>
   </si>
   <si>
@@ -620,6 +611,9 @@
   </si>
   <si>
     <t>2.3</t>
+  </si>
+  <si>
+    <t>discrimi</t>
   </si>
 </sst>
 </file>
@@ -705,7 +699,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="319">
+  <cellStyleXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1025,8 +1019,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1036,7 +1034,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1048,7 +1045,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="319">
+  <cellStyles count="323">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1208,6 +1205,8 @@
     <cellStyle name="Gevolgde hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1367,6 +1366,8 @@
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1699,7 +1700,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="A1:J36"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1714,57 +1715,60 @@
     <col min="8" max="8" width="12.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.75" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="1"/>
+    <col min="11" max="11" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" s="9"/>
+      <c r="K1" s="13" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>138</v>
+        <v>83</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>33</v>
@@ -1776,11 +1780,14 @@
         <v>2165</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" s="15">
+        <v>169</v>
+      </c>
+      <c r="J2" s="14">
         <f>0.049*(0.845*G2)</f>
         <v>355458.86103000003</v>
+      </c>
+      <c r="K2" s="5">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1788,16 +1795,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>137</v>
+        <v>64</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>34</v>
@@ -1809,11 +1816,14 @@
         <v>2092</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J3" s="15">
+        <v>170</v>
+      </c>
+      <c r="J3" s="14">
         <f>0.073*(0.845*G3)</f>
         <v>694476.50129000004</v>
+      </c>
+      <c r="K3" s="5">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1821,19 +1831,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="11">
+        <v>65</v>
+      </c>
+      <c r="D4" s="10">
         <v>14</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
+      <c r="E4" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="2">
+        <v>31.42</v>
       </c>
       <c r="G4" s="3">
         <v>7202198</v>
@@ -1842,11 +1852,14 @@
         <v>324</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" s="15">
+        <v>171</v>
+      </c>
+      <c r="J4" s="14">
         <f>0.17*(0.845*G4)</f>
         <v>1034595.7427000001</v>
+      </c>
+      <c r="K4" s="5">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1854,32 +1867,35 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="11">
+        <v>74</v>
+      </c>
+      <c r="D5" s="10">
         <v>14</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>139</v>
+      <c r="E5" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3">
         <v>4225316</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>755</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="I5" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="14">
         <f>0.146*(0.845*G5)</f>
         <v>521277.23491999996</v>
+      </c>
+      <c r="K5" s="5">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1887,19 +1903,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>140</v>
+        <v>76</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="3">
         <v>847008</v>
@@ -1907,12 +1923,15 @@
       <c r="H6" s="5">
         <v>2223</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J6" s="14">
         <f>0.14*(0.845*G6)</f>
         <v>100201.04640000001</v>
+      </c>
+      <c r="K6" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1920,19 +1939,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>141</v>
+        <v>66</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3">
         <v>10538275</v>
@@ -1941,11 +1960,14 @@
         <v>725</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="J7" s="15">
+        <v>173</v>
+      </c>
+      <c r="J7" s="14">
         <f>0.054*(0.845*G7)</f>
         <v>480861.48824999999</v>
+      </c>
+      <c r="K7" s="5">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1953,19 +1975,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>142</v>
+        <v>67</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="3">
         <v>5659715</v>
@@ -1973,12 +1995,15 @@
       <c r="H8" s="6">
         <v>2389</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="J8" s="15">
+      <c r="I8" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="14">
         <f>0.055*(0.845*G8)</f>
         <v>263035.254625</v>
+      </c>
+      <c r="K8" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1986,19 +2011,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>143</v>
+        <v>69</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3">
         <v>1313271</v>
@@ -2006,12 +2031,15 @@
       <c r="H9" s="2">
         <v>832</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" s="14">
         <f>0.067*(0.845*G9)</f>
         <v>74350.837664999999</v>
+      </c>
+      <c r="K9" s="5">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2019,19 +2047,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>144</v>
+        <v>89</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3">
         <v>5471753</v>
@@ -2039,12 +2067,15 @@
       <c r="H10" s="2">
         <v>2479</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="I10" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="14">
         <f>0.07*(0.845*G10)</f>
         <v>323654.18995000003</v>
+      </c>
+      <c r="K10" s="5">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2052,19 +2083,19 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="11">
+        <v>73</v>
+      </c>
+      <c r="D11" s="10">
         <v>13</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>145</v>
+      <c r="E11" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="3">
         <v>66352469</v>
@@ -2072,12 +2103,15 @@
       <c r="H11" s="2">
         <v>2183</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="J11" s="15">
+      <c r="I11" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="J11" s="14">
         <f>0.088*(0.845*G11)</f>
         <v>4933969.5948399995</v>
+      </c>
+      <c r="K11" s="5">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2085,19 +2119,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="11">
+        <v>68</v>
+      </c>
+      <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>146</v>
+      <c r="E12" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="3">
         <v>81174000</v>
@@ -2106,44 +2140,50 @@
         <v>2155</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J12" s="15">
+        <v>177</v>
+      </c>
+      <c r="J12" s="14">
         <f>0.047*(0.845*G12)</f>
         <v>3223825.41</v>
       </c>
+      <c r="K12" s="5">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>147</v>
+        <v>71</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="3">
         <v>10812467</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <v>1262</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="J13" s="15">
+      <c r="I13" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="14">
         <f>0.248*(0.845*G13)</f>
         <v>2265860.58452</v>
+      </c>
+      <c r="K13" s="5">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2151,32 +2191,35 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="11">
+        <v>80</v>
+      </c>
+      <c r="D14" s="10">
         <v>8</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>148</v>
+      <c r="E14" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" s="3">
         <v>9849000</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <v>532</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J14" s="15">
+      <c r="I14" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J14" s="14">
         <f>0.067*(0.845*G14)</f>
         <v>557601.13500000001</v>
+      </c>
+      <c r="K14" s="5">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2184,32 +2227,35 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="11">
+        <v>92</v>
+      </c>
+      <c r="D15" s="10">
         <v>6</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15" s="3">
         <v>329100</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="12">
         <v>2334</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="J15" s="15">
+      <c r="I15" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" s="14">
         <f>0.039*(0.845*G15)</f>
         <v>10845.4905</v>
+      </c>
+      <c r="K15" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2217,85 +2263,91 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="11">
+        <v>70</v>
+      </c>
+      <c r="D16" s="10">
         <v>13</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>145</v>
+      <c r="E16" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G16" s="3">
         <v>4625885</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="12">
         <v>2186</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J16" s="15">
+        <v>171</v>
+      </c>
+      <c r="J16" s="14">
         <f>0.1*(0.845*G16)</f>
         <v>390887.28249999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>149</v>
+        <v>75</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3">
         <v>60795612</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="12">
         <v>2030</v>
       </c>
-      <c r="I17" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="J17" s="15">
+      <c r="I17" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="J17" s="14">
         <f>0.16*(0.845*G17)</f>
         <v>8219566.7423999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="11">
+        <v>77</v>
+      </c>
+      <c r="D18" s="10">
         <v>16</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>36</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G18" s="3">
         <v>1986096</v>
@@ -2303,98 +2355,107 @@
       <c r="H18" s="2">
         <v>379</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="J18" s="15">
+      <c r="I18" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J18" s="14">
         <f>0.1*(0.845*G18)</f>
         <v>167825.11199999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>158</v>
+        <v>93</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G19" s="3">
         <v>37369</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="12">
         <v>5314</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J19" s="15">
+      <c r="I19" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19" s="14">
         <f>0.023*(0.845*G19)</f>
         <v>726.26651500000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>140</v>
+        <v>78</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3">
         <v>2921262</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="12">
         <v>496</v>
       </c>
-      <c r="I20" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="J20" s="15">
+      <c r="I20" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" s="14">
         <f>0.099*(0.845*G20)</f>
         <v>244378.17261000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>150</v>
+        <v>79</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G21" s="3">
         <v>562958</v>
@@ -2402,65 +2463,71 @@
       <c r="H21" s="6">
         <v>3187</v>
       </c>
-      <c r="I21" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="J21" s="15">
+      <c r="I21" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="14">
         <f>0.05*(0.845*G21)</f>
         <v>23784.9755</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="11">
+        <v>81</v>
+      </c>
+      <c r="D22" s="10">
         <v>7</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22" s="3">
         <v>429344</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="12">
         <v>1006</v>
       </c>
-      <c r="I22" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="J22" s="15">
+      <c r="I22" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="J22" s="14">
         <f>0.048*(0.845*G22)</f>
         <v>17414.192640000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>151</v>
+        <v>96</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" s="3">
         <v>622099</v>
@@ -2468,32 +2535,35 @@
       <c r="H23" s="5">
         <v>726</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="J23" s="15">
+      <c r="I23" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J23" s="14">
         <f>0.145*(0.845*G23)</f>
         <v>76222.679974999992</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="11">
+        <v>82</v>
+      </c>
+      <c r="D24" s="10">
         <v>7</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>28</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G24" s="3">
         <v>16900726</v>
@@ -2501,32 +2571,35 @@
       <c r="H24" s="6">
         <v>2158</v>
       </c>
-      <c r="I24" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J24" s="15">
+      <c r="I24" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J24" s="14">
         <f>0.065*(0.845*G24)</f>
         <v>928272.37555</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>152</v>
+        <v>94</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G25" s="3">
         <v>5165802</v>
@@ -2534,32 +2607,35 @@
       <c r="H25" s="5">
         <v>3850</v>
       </c>
-      <c r="I25" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="J25" s="15">
+      <c r="I25" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="J25" s="14">
         <f>0.028*(0.845*G25)</f>
         <v>122222.87531999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>153</v>
+        <v>84</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G26" s="3">
         <v>38005614</v>
@@ -2567,94 +2643,103 @@
       <c r="H26" s="5">
         <v>634</v>
       </c>
-      <c r="I26" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="J26" s="15">
+      <c r="I26" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="J26" s="14">
         <f>0.077*(0.845*G26)</f>
         <v>2472835.2749099997</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="11">
+        <v>85</v>
+      </c>
+      <c r="D27" s="10">
         <v>16</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>154</v>
+      <c r="E27" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G27" s="3">
         <v>10374822</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="13">
         <v>1056</v>
       </c>
-      <c r="I27" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="J27" s="15">
+      <c r="I27" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="J27" s="14">
         <f>0.125*(0.845*G27)</f>
         <v>1095840.57375</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="11">
+        <v>86</v>
+      </c>
+      <c r="D28" s="10">
         <v>6</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>155</v>
+      <c r="E28" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G28" s="3">
         <v>19861408</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="13">
         <v>345</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="J28" s="15">
+      <c r="I28" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="J28" s="14">
         <f>0.055*(0.845*G28)</f>
         <v>923058.93679999991</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="11">
+        <v>97</v>
+      </c>
+      <c r="D29" s="10">
         <v>10</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>30</v>
       </c>
       <c r="F29" s="2">
@@ -2666,98 +2751,107 @@
       <c r="H29" s="5">
         <v>377</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="J29" s="15">
+      <c r="I29" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J29" s="14">
         <f>0.2*(0.845*G29)</f>
         <v>1183000</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>156</v>
+        <v>88</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G30" s="3">
         <v>5421349</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <v>664</v>
       </c>
-      <c r="I30" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="J30" s="15">
+      <c r="I30" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="J30" s="14">
         <f>0.118*(0.845*G30)</f>
         <v>540562.70878999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="11">
+        <v>87</v>
+      </c>
+      <c r="D31" s="10">
         <v>5</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>157</v>
+      <c r="E31" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G31" s="3">
         <v>2062874</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <v>1023</v>
       </c>
-      <c r="I31" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" s="15">
+      <c r="I31" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J31" s="14">
         <f>0.089*(0.845*G31)</f>
         <v>155138.43917</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="11">
+        <v>72</v>
+      </c>
+      <c r="D32" s="10">
         <v>16</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <v>36</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>43</v>
+      <c r="F32" s="2">
+        <v>6.4</v>
       </c>
       <c r="G32" s="3">
         <v>46439864</v>
@@ -2766,31 +2860,34 @@
         <v>1702</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="J32" s="15">
+        <v>176</v>
+      </c>
+      <c r="J32" s="14">
         <f>0.223*(0.845*G32)</f>
         <v>8750895.7728399988</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="11">
+        <v>90</v>
+      </c>
+      <c r="D33" s="10">
         <v>6</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>155</v>
+      <c r="E33" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G33" s="3">
         <v>9747355</v>
@@ -2798,32 +2895,35 @@
       <c r="H33" s="5">
         <v>2825</v>
       </c>
-      <c r="I33" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="J33" s="15">
+      <c r="I33" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="J33" s="14">
         <f>0.057*(0.845*G33)</f>
         <v>469481.35357500002</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>158</v>
+        <v>95</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34" s="3">
         <v>8236573</v>
@@ -2831,81 +2931,93 @@
       <c r="H34" s="5">
         <v>2930</v>
       </c>
-      <c r="I34" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J34" s="15">
+      <c r="I34" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J34" s="14">
         <f>0.034*(0.845*G34)</f>
         <v>236636.74228999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="11">
+        <v>98</v>
+      </c>
+      <c r="D35" s="10">
         <v>20</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="9">
         <v>40</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>63</v>
+      <c r="F35" s="2">
+        <v>45.87</v>
       </c>
       <c r="G35" s="3">
         <v>77695904</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="13">
         <v>510</v>
       </c>
-      <c r="I35" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="J35" s="15">
+      <c r="I35" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J35" s="14">
         <f>0.083*(0.845*G35)</f>
         <v>5449202.2270400003</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="11">
+        <v>91</v>
+      </c>
+      <c r="D36" s="10">
         <v>10</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="9">
         <v>30.2</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G36" s="3">
         <v>64767115</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="13">
         <v>2233</v>
       </c>
-      <c r="I36" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="J36" s="15">
+      <c r="I36" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="J36" s="14">
         <f>0.044*(0.845*G36)</f>
         <v>2408041.3356999997</v>
       </c>
+      <c r="K36" s="5">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K36">
+    <sortCondition ref="C2:C36"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
add country names ++ variablesUI update ++ add variablesScale ++ add displayCurrentType ++ box-sizingbox ++ update icons-set
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1700,7 +1700,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1756,71 +1756,71 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>160</v>
+        <v>65</v>
+      </c>
+      <c r="D2" s="10">
+        <v>14</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>136</v>
+      </c>
+      <c r="F2" s="2">
+        <v>31.42</v>
       </c>
       <c r="G2" s="3">
-        <v>8584926</v>
+        <v>7202198</v>
       </c>
       <c r="H2" s="2">
-        <v>2165</v>
+        <v>324</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J2" s="14">
-        <f>0.049*(0.845*G2)</f>
-        <v>355458.86103000003</v>
+        <f>0.17*(0.845*G2)</f>
+        <v>1034595.7427000001</v>
       </c>
       <c r="K2" s="5">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>156</v>
+        <v>86</v>
+      </c>
+      <c r="D3" s="10">
+        <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G3" s="3">
-        <v>11258434</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2092</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>170</v>
+        <v>19861408</v>
+      </c>
+      <c r="H3" s="13">
+        <v>345</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="J3" s="14">
-        <f>0.073*(0.845*G3)</f>
-        <v>694476.50129000004</v>
+        <f>0.055*(0.845*G3)</f>
+        <v>923058.93679999991</v>
       </c>
       <c r="K3" s="5">
         <v>78</v>
@@ -1828,85 +1828,85 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D4" s="10">
-        <v>14</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>136</v>
+        <v>10</v>
+      </c>
+      <c r="E4" s="9">
+        <v>30</v>
       </c>
       <c r="F4" s="2">
-        <v>31.42</v>
+        <v>25.05</v>
       </c>
       <c r="G4" s="3">
-        <v>7202198</v>
-      </c>
-      <c r="H4" s="2">
-        <v>324</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>171</v>
+        <v>7000000</v>
+      </c>
+      <c r="H4" s="5">
+        <v>377</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="J4" s="14">
-        <f>0.17*(0.845*G4)</f>
-        <v>1034595.7427000001</v>
+        <f>0.2*(0.845*G4)</f>
+        <v>1183000</v>
       </c>
       <c r="K4" s="5">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D5" s="10">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>136</v>
+        <v>16</v>
+      </c>
+      <c r="E5" s="9">
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3">
-        <v>4225316</v>
-      </c>
-      <c r="H5" s="12">
-        <v>755</v>
+        <v>1986096</v>
+      </c>
+      <c r="H5" s="2">
+        <v>379</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="J5" s="14">
-        <f>0.146*(0.845*G5)</f>
-        <v>521277.23491999996</v>
+        <f>0.1*(0.845*G5)</f>
+        <v>167825.11199999999</v>
       </c>
       <c r="K5" s="5">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>162</v>
@@ -1915,1108 +1915,1108 @@
         <v>137</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3">
-        <v>847008</v>
-      </c>
-      <c r="H6" s="5">
-        <v>2223</v>
+        <v>2921262</v>
+      </c>
+      <c r="H6" s="12">
+        <v>496</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J6" s="14">
-        <f>0.14*(0.845*G6)</f>
-        <v>100201.04640000001</v>
+        <f>0.099*(0.845*G6)</f>
+        <v>244378.17261000004</v>
       </c>
       <c r="K6" s="5">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>98</v>
+      </c>
+      <c r="D7" s="10">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45.87</v>
       </c>
       <c r="G7" s="3">
-        <v>10538275</v>
-      </c>
-      <c r="H7" s="6">
-        <v>725</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>173</v>
+        <v>77695904</v>
+      </c>
+      <c r="H7" s="13">
+        <v>510</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="J7" s="14">
-        <f>0.054*(0.845*G7)</f>
-        <v>480861.48824999999</v>
+        <f>0.083*(0.845*G7)</f>
+        <v>5449202.2270400003</v>
       </c>
       <c r="K7" s="5">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="D8" s="10">
+        <v>8</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G8" s="3">
-        <v>5659715</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2389</v>
+        <v>9849000</v>
+      </c>
+      <c r="H8" s="12">
+        <v>532</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="J8" s="14">
-        <f>0.055*(0.845*G8)</f>
-        <v>263035.254625</v>
+        <f>0.067*(0.845*G8)</f>
+        <v>557601.13500000001</v>
       </c>
       <c r="K8" s="5">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>162</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="G9" s="3">
-        <v>1313271</v>
-      </c>
-      <c r="H9" s="2">
-        <v>832</v>
+        <v>38005614</v>
+      </c>
+      <c r="H9" s="5">
+        <v>634</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="J9" s="14">
-        <f>0.067*(0.845*G9)</f>
-        <v>74350.837664999999</v>
+        <f>0.077*(0.845*G9)</f>
+        <v>2472835.2749099997</v>
       </c>
       <c r="K9" s="5">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G10" s="3">
-        <v>5471753</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2479</v>
+        <v>5421349</v>
+      </c>
+      <c r="H10" s="13">
+        <v>664</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="J10" s="14">
-        <f>0.07*(0.845*G10)</f>
-        <v>323654.18995000003</v>
+        <f>0.118*(0.845*G10)</f>
+        <v>540562.70878999995</v>
       </c>
       <c r="K10" s="5">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="10">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G11" s="3">
-        <v>66352469</v>
-      </c>
-      <c r="H11" s="2">
-        <v>2183</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>176</v>
+        <v>10538275</v>
+      </c>
+      <c r="H11" s="6">
+        <v>725</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="J11" s="14">
-        <f>0.088*(0.845*G11)</f>
-        <v>4933969.5948399995</v>
+        <f>0.054*(0.845*G11)</f>
+        <v>480861.48824999999</v>
       </c>
       <c r="K11" s="5">
-        <v>77</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>166</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="10">
-        <v>10</v>
+        <v>96</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G12" s="3">
-        <v>81174000</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2155</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>177</v>
+        <v>622099</v>
+      </c>
+      <c r="H12" s="5">
+        <v>726</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="J12" s="14">
-        <f>0.047*(0.845*G12)</f>
-        <v>3223825.41</v>
+        <f>0.145*(0.845*G12)</f>
+        <v>76222.679974999992</v>
       </c>
       <c r="K12" s="5">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>164</v>
+        <v>74</v>
+      </c>
+      <c r="D13" s="10">
+        <v>14</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G13" s="3">
-        <v>10812467</v>
+        <v>4225316</v>
       </c>
       <c r="H13" s="12">
-        <v>1262</v>
+        <v>755</v>
       </c>
       <c r="I13" s="13" t="s">
         <v>172</v>
       </c>
       <c r="J13" s="14">
-        <f>0.248*(0.845*G13)</f>
-        <v>2265860.58452</v>
+        <f>0.146*(0.845*G13)</f>
+        <v>521277.23491999996</v>
       </c>
       <c r="K13" s="5">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="10">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G14" s="3">
-        <v>9849000</v>
-      </c>
-      <c r="H14" s="12">
-        <v>532</v>
+        <v>1313271</v>
+      </c>
+      <c r="H14" s="2">
+        <v>832</v>
       </c>
       <c r="I14" s="13" t="s">
         <v>174</v>
       </c>
       <c r="J14" s="14">
         <f>0.067*(0.845*G14)</f>
-        <v>557601.13500000001</v>
+        <v>74350.837664999999</v>
       </c>
       <c r="K14" s="5">
-        <v>83</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>130</v>
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D15" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" s="9">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G15" s="3">
-        <v>329100</v>
+        <v>429344</v>
       </c>
       <c r="H15" s="12">
-        <v>2334</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>169</v>
+        <v>1006</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="J15" s="14">
-        <f>0.039*(0.845*G15)</f>
-        <v>10845.4905</v>
+        <f>0.048*(0.845*G15)</f>
+        <v>17414.192640000001</v>
       </c>
       <c r="K15" s="5">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D16" s="10">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="G16" s="3">
-        <v>4625885</v>
-      </c>
-      <c r="H16" s="12">
-        <v>2186</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>171</v>
+        <v>2062874</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1023</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="J16" s="14">
-        <f>0.1*(0.845*G16)</f>
-        <v>390887.28249999997</v>
+        <f>0.089*(0.845*G16)</f>
+        <v>155138.43917</v>
       </c>
       <c r="K16" s="5">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>163</v>
-      </c>
       <c r="E17" s="9" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G17" s="3">
-        <v>60795612</v>
-      </c>
-      <c r="H17" s="12">
-        <v>2030</v>
+        <v>10374822</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1056</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>176</v>
       </c>
       <c r="J17" s="14">
-        <f>0.16*(0.845*G17)</f>
-        <v>8219566.7423999999</v>
+        <f>0.125*(0.845*G17)</f>
+        <v>1095840.57375</v>
       </c>
       <c r="K17" s="5">
-        <v>61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="10">
-        <v>16</v>
-      </c>
-      <c r="E18" s="9">
-        <v>36</v>
+        <v>71</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G18" s="3">
-        <v>1986096</v>
-      </c>
-      <c r="H18" s="2">
-        <v>379</v>
+        <v>10812467</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1262</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J18" s="14">
-        <f>0.1*(0.845*G18)</f>
-        <v>167825.11199999999</v>
+        <f>0.248*(0.845*G18)</f>
+        <v>2265860.58452</v>
       </c>
       <c r="K18" s="5">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="10">
+        <v>16</v>
+      </c>
+      <c r="E19" s="9">
+        <v>36</v>
+      </c>
+      <c r="F19" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="G19" s="3">
+        <v>46439864</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1702</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" s="14">
+        <f>0.223*(0.845*G19)</f>
+        <v>8750895.7728399988</v>
+      </c>
+      <c r="K19" s="5">
         <v>49</v>
-      </c>
-      <c r="G19" s="3">
-        <v>37369</v>
-      </c>
-      <c r="H19" s="12">
-        <v>5314</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="J19" s="14">
-        <f>0.023*(0.845*G19)</f>
-        <v>726.26651500000003</v>
-      </c>
-      <c r="K19" s="5">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G20" s="3">
-        <v>2921262</v>
+        <v>60795612</v>
       </c>
       <c r="H20" s="12">
-        <v>496</v>
+        <v>2030</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J20" s="14">
-        <f>0.099*(0.845*G20)</f>
-        <v>244378.17261000004</v>
+        <f>0.16*(0.845*G20)</f>
+        <v>8219566.7423999999</v>
       </c>
       <c r="K20" s="5">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G21" s="3">
-        <v>562958</v>
+        <v>11258434</v>
       </c>
       <c r="H21" s="6">
-        <v>3187</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>172</v>
+        <v>2092</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="J21" s="14">
-        <f>0.05*(0.845*G21)</f>
-        <v>23784.9755</v>
+        <f>0.073*(0.845*G21)</f>
+        <v>694476.50129000004</v>
       </c>
       <c r="K21" s="5">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>81</v>
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D22" s="10">
-        <v>7</v>
-      </c>
-      <c r="E22" s="9">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G22" s="3">
-        <v>429344</v>
-      </c>
-      <c r="H22" s="12">
-        <v>1006</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>180</v>
+        <v>81174000</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2155</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="J22" s="14">
-        <f>0.048*(0.845*G22)</f>
-        <v>17414.192640000001</v>
+        <f>0.047*(0.845*G22)</f>
+        <v>3223825.41</v>
       </c>
       <c r="K22" s="5">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>148</v>
+        <v>82</v>
+      </c>
+      <c r="D23" s="10">
+        <v>7</v>
+      </c>
+      <c r="E23" s="9">
+        <v>28</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G23" s="3">
-        <v>622099</v>
-      </c>
-      <c r="H23" s="5">
-        <v>726</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>181</v>
+        <v>16900726</v>
+      </c>
+      <c r="H23" s="6">
+        <v>2158</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="J23" s="14">
-        <f>0.145*(0.845*G23)</f>
-        <v>76222.679974999992</v>
+        <f>0.065*(0.845*G23)</f>
+        <v>928272.37555</v>
       </c>
       <c r="K23" s="5">
-        <v>50</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="10">
-        <v>7</v>
-      </c>
-      <c r="E24" s="9">
-        <v>28</v>
+        <v>83</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="G24" s="3">
-        <v>16900726</v>
-      </c>
-      <c r="H24" s="6">
-        <v>2158</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>174</v>
+        <v>8584926</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2165</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="J24" s="14">
-        <f>0.065*(0.845*G24)</f>
-        <v>928272.37555</v>
+        <f>0.049*(0.845*G24)</f>
+        <v>355458.86103000003</v>
       </c>
       <c r="K24" s="5">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>159</v>
+        <v>73</v>
+      </c>
+      <c r="D25" s="10">
+        <v>13</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G25" s="3">
-        <v>5165802</v>
-      </c>
-      <c r="H25" s="5">
-        <v>3850</v>
+        <v>66352469</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2183</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="J25" s="14">
-        <f>0.028*(0.845*G25)</f>
-        <v>122222.87531999999</v>
+        <f>0.088*(0.845*G25)</f>
+        <v>4933969.5948399995</v>
       </c>
       <c r="K25" s="5">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>162</v>
+        <v>70</v>
+      </c>
+      <c r="D26" s="10">
+        <v>13</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G26" s="3">
-        <v>38005614</v>
-      </c>
-      <c r="H26" s="5">
-        <v>634</v>
-      </c>
-      <c r="I26" s="13" t="s">
-        <v>183</v>
+        <v>4625885</v>
+      </c>
+      <c r="H26" s="12">
+        <v>2186</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="J26" s="14">
-        <f>0.077*(0.845*G26)</f>
-        <v>2472835.2749099997</v>
+        <f>0.1*(0.845*G26)</f>
+        <v>390887.28249999997</v>
       </c>
       <c r="K26" s="5">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>85</v>
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="10">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="G27" s="3">
-        <v>10374822</v>
-      </c>
-      <c r="H27" s="13">
-        <v>1056</v>
+        <v>847008</v>
+      </c>
+      <c r="H27" s="5">
+        <v>2223</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J27" s="14">
-        <f>0.125*(0.845*G27)</f>
-        <v>1095840.57375</v>
+        <f>0.14*(0.845*G27)</f>
+        <v>100201.04640000001</v>
       </c>
       <c r="K27" s="5">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D28" s="10">
-        <v>6</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="E28" s="9">
+        <v>30.2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G28" s="3">
-        <v>19861408</v>
+        <v>64767115</v>
       </c>
       <c r="H28" s="13">
-        <v>345</v>
+        <v>2233</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="J28" s="14">
-        <f>0.055*(0.845*G28)</f>
-        <v>923058.93679999991</v>
+        <f>0.044*(0.845*G28)</f>
+        <v>2408041.3356999997</v>
       </c>
       <c r="K28" s="5">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D29" s="10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E29" s="9">
-        <v>30</v>
-      </c>
-      <c r="F29" s="2">
-        <v>25.05</v>
+        <v>27</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G29" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="H29" s="5">
-        <v>377</v>
+        <v>329100</v>
+      </c>
+      <c r="H29" s="12">
+        <v>2334</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="J29" s="14">
-        <f>0.2*(0.845*G29)</f>
-        <v>1183000</v>
+        <f>0.039*(0.845*G29)</f>
+        <v>10845.4905</v>
       </c>
       <c r="K29" s="5">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>158</v>
+        <v>47</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="G30" s="3">
-        <v>5421349</v>
-      </c>
-      <c r="H30" s="13">
-        <v>664</v>
+        <v>5659715</v>
+      </c>
+      <c r="H30" s="6">
+        <v>2389</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="J30" s="14">
-        <f>0.118*(0.845*G30)</f>
-        <v>540562.70878999995</v>
+        <f>0.055*(0.845*G30)</f>
+        <v>263035.254625</v>
       </c>
       <c r="K30" s="5">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="10">
-        <v>5</v>
+        <v>89</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G31" s="3">
-        <v>2062874</v>
-      </c>
-      <c r="H31" s="13">
-        <v>1023</v>
+        <v>5471753</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2479</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>175</v>
       </c>
       <c r="J31" s="14">
-        <f>0.089*(0.845*G31)</f>
-        <v>155138.43917</v>
+        <f>0.07*(0.845*G31)</f>
+        <v>323654.18995000003</v>
       </c>
       <c r="K31" s="5">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D32" s="10">
-        <v>16</v>
-      </c>
-      <c r="E32" s="9">
-        <v>36</v>
-      </c>
-      <c r="F32" s="2">
-        <v>6.4</v>
+        <v>6</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="G32" s="3">
-        <v>46439864</v>
+        <v>9747355</v>
       </c>
       <c r="H32" s="5">
-        <v>1702</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>176</v>
+        <v>2825</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="J32" s="14">
-        <f>0.223*(0.845*G32)</f>
-        <v>8750895.7728399988</v>
+        <f>0.057*(0.845*G32)</f>
+        <v>469481.35357500002</v>
       </c>
       <c r="K32" s="5">
-        <v>49</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="3" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="10">
-        <v>6</v>
+        <v>95</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="G33" s="3">
-        <v>9747355</v>
+        <v>8236573</v>
       </c>
       <c r="H33" s="5">
-        <v>2825</v>
+        <v>2930</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="J33" s="14">
-        <f>0.057*(0.845*G33)</f>
-        <v>469481.35357500002</v>
+        <f>0.034*(0.845*G33)</f>
+        <v>236636.74228999999</v>
       </c>
       <c r="K33" s="5">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G34" s="3">
-        <v>8236573</v>
-      </c>
-      <c r="H34" s="5">
-        <v>2930</v>
+        <v>562958</v>
+      </c>
+      <c r="H34" s="6">
+        <v>3187</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J34" s="14">
-        <f>0.034*(0.845*G34)</f>
-        <v>236636.74228999999</v>
+        <f>0.05*(0.845*G34)</f>
+        <v>23784.9755</v>
       </c>
       <c r="K34" s="5">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="10">
-        <v>20</v>
-      </c>
-      <c r="E35" s="9">
-        <v>40</v>
-      </c>
-      <c r="F35" s="2">
-        <v>45.87</v>
+        <v>94</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="G35" s="3">
-        <v>77695904</v>
-      </c>
-      <c r="H35" s="13">
-        <v>510</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>181</v>
+        <v>5165802</v>
+      </c>
+      <c r="H35" s="5">
+        <v>3850</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="J35" s="14">
-        <f>0.083*(0.845*G35)</f>
-        <v>5449202.2270400003</v>
+        <f>0.028*(0.845*G35)</f>
+        <v>122222.87531999999</v>
       </c>
       <c r="K35" s="5">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="3">
+        <v>37369</v>
+      </c>
+      <c r="H36" s="12">
+        <v>5314</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J36" s="14">
+        <f>0.023*(0.845*G36)</f>
+        <v>726.26651500000003</v>
+      </c>
+      <c r="K36" s="5">
         <v>31</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D36" s="10">
-        <v>10</v>
-      </c>
-      <c r="E36" s="9">
-        <v>30.2</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="3">
-        <v>64767115</v>
-      </c>
-      <c r="H36" s="13">
-        <v>2233</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="J36" s="14">
-        <f>0.044*(0.845*G36)</f>
-        <v>2408041.3356999997</v>
-      </c>
-      <c r="K36" s="5">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:K36">
-    <sortCondition ref="C2:C36"/>
+    <sortCondition ref="H2:H36"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
update data ++ add fonts ++ add sidebar feature ++ add explain ++ add sidebar
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>AT</t>
   </si>
@@ -154,93 +154,6 @@
     <t>LI</t>
   </si>
   <si>
-    <t>10.01</t>
-  </si>
-  <si>
-    <t>12.8</t>
-  </si>
-  <si>
-    <t>10.47</t>
-  </si>
-  <si>
-    <t>14.45</t>
-  </si>
-  <si>
-    <t>10.07</t>
-  </si>
-  <si>
-    <t>10.23</t>
-  </si>
-  <si>
-    <t>7.43</t>
-  </si>
-  <si>
-    <t>9.63</t>
-  </si>
-  <si>
-    <t>20.63</t>
-  </si>
-  <si>
-    <t>21.89</t>
-  </si>
-  <si>
-    <t>31.33</t>
-  </si>
-  <si>
-    <t>26.82</t>
-  </si>
-  <si>
-    <t>26.73</t>
-  </si>
-  <si>
-    <t>10.87</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>23.75</t>
-  </si>
-  <si>
-    <t>7.02</t>
-  </si>
-  <si>
-    <t>19.2</t>
-  </si>
-  <si>
-    <t>6.7</t>
-  </si>
-  <si>
-    <t>21.1</t>
-  </si>
-  <si>
-    <t>6.46</t>
-  </si>
-  <si>
-    <t>6.52</t>
-  </si>
-  <si>
-    <t>11.03</t>
-  </si>
-  <si>
-    <t>17.73</t>
-  </si>
-  <si>
-    <t>23.48</t>
-  </si>
-  <si>
-    <t>8.98</t>
-  </si>
-  <si>
-    <t>20.38</t>
-  </si>
-  <si>
-    <t>11.39</t>
-  </si>
-  <si>
-    <t>19.93</t>
-  </si>
-  <si>
     <t>freedom</t>
   </si>
   <si>
@@ -457,99 +370,6 @@
     <t>gemiddeld-ink</t>
   </si>
   <si>
-    <t>28.4</t>
-  </si>
-  <si>
-    <t>30.8</t>
-  </si>
-  <si>
-    <t>34.2</t>
-  </si>
-  <si>
-    <t>32.6</t>
-  </si>
-  <si>
-    <t>26.4</t>
-  </si>
-  <si>
-    <t>29.5</t>
-  </si>
-  <si>
-    <t>32.7</t>
-  </si>
-  <si>
-    <t>27.6</t>
-  </si>
-  <si>
-    <t>33.3</t>
-  </si>
-  <si>
-    <t>30.1</t>
-  </si>
-  <si>
-    <t>35.7</t>
-  </si>
-  <si>
-    <t>28.9</t>
-  </si>
-  <si>
-    <t>34.5</t>
-  </si>
-  <si>
-    <t>32.4</t>
-  </si>
-  <si>
-    <t>30.6</t>
-  </si>
-  <si>
-    <t>25.5</t>
-  </si>
-  <si>
-    <t>32.8</t>
-  </si>
-  <si>
-    <t>36.3</t>
-  </si>
-  <si>
-    <t>27.2</t>
-  </si>
-  <si>
-    <t>26.5</t>
-  </si>
-  <si>
-    <t>24.9</t>
-  </si>
-  <si>
-    <t>31.8</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>6.5</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>10.5</t>
-  </si>
-  <si>
-    <t>11.5</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
-    <t>14.5</t>
-  </si>
-  <si>
-    <t>15.5</t>
-  </si>
-  <si>
     <t>gini</t>
   </si>
   <si>
@@ -560,57 +380,6 @@
   </si>
   <si>
     <t>werkloosheid</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>2.8</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>2.6</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>2.3</t>
   </si>
   <si>
     <t>discrimi</t>
@@ -623,12 +392,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -678,6 +448,20 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -702,7 +486,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="389">
+  <cellStyleXfs count="449">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1092,8 +876,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1114,8 +958,20 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="389">
+  <cellStyles count="449">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1310,6 +1166,36 @@
     <cellStyle name="Gevolgde hyperlink" xfId="384" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="386" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="448" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1504,6 +1390,36 @@
     <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1833,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1856,63 +1772,65 @@
     <col min="13" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>186</v>
+        <v>109</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>187</v>
+        <v>110</v>
       </c>
       <c r="M1" s="14"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1"/>
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>54</v>
+      </c>
+      <c r="D2" s="23">
+        <v>10.5</v>
+      </c>
+      <c r="E2" s="22">
+        <v>30.8</v>
+      </c>
+      <c r="F2" s="17">
+        <v>10.01</v>
       </c>
       <c r="G2" s="3">
         <v>8584926</v>
@@ -1920,8 +1838,8 @@
       <c r="H2" s="2">
         <v>2165</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>169</v>
+      <c r="I2" s="21">
+        <v>1.6</v>
       </c>
       <c r="J2" s="13">
         <f>0.049*(0.845*G2)</f>
@@ -1933,25 +1851,26 @@
       <c r="L2" s="5">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D3" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="E3" s="22">
+        <v>28.4</v>
+      </c>
+      <c r="F3" s="17">
+        <v>12.8</v>
       </c>
       <c r="G3" s="3">
         <v>11258434</v>
@@ -1959,8 +1878,8 @@
       <c r="H3" s="15">
         <v>2092</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>170</v>
+      <c r="I3" s="21">
+        <v>2.4</v>
       </c>
       <c r="J3" s="13">
         <f>0.073*(0.845*G3)</f>
@@ -1972,24 +1891,25 @@
       <c r="L3" s="5">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D4" s="9">
         <v>14</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="22">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="F4" s="17">
         <v>31.42</v>
       </c>
       <c r="G4" s="3">
@@ -1998,8 +1918,8 @@
       <c r="H4" s="2">
         <v>324</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>171</v>
+      <c r="I4" s="21">
+        <v>0.7</v>
       </c>
       <c r="J4" s="13">
         <f>0.17*(0.845*G4)</f>
@@ -2011,25 +1931,26 @@
       <c r="L4" s="5">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D5" s="9">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>44</v>
+      <c r="E5" s="22">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="F5" s="17">
+        <v>26.82</v>
       </c>
       <c r="G5" s="3">
         <v>4225316</v>
@@ -2037,8 +1958,8 @@
       <c r="H5" s="11">
         <v>755</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>172</v>
+      <c r="I5" s="19">
+        <v>1</v>
       </c>
       <c r="J5" s="13">
         <f>0.146*(0.845*G5)</f>
@@ -2050,25 +1971,26 @@
       <c r="L5" s="5">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="D6" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E6" s="22">
+        <v>32.6</v>
+      </c>
+      <c r="F6" s="17">
+        <v>29.54</v>
       </c>
       <c r="G6" s="3">
         <v>847008</v>
@@ -2076,8 +1998,8 @@
       <c r="H6" s="5">
         <v>2223</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>173</v>
+      <c r="I6" s="19">
+        <v>1.2</v>
       </c>
       <c r="J6" s="13">
         <f>0.14*(0.845*G6)</f>
@@ -2089,25 +2011,26 @@
       <c r="L6" s="5">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="D7" s="23">
+        <v>5.5</v>
+      </c>
+      <c r="E7" s="22">
+        <v>26.4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>10.07</v>
       </c>
       <c r="G7" s="3">
         <v>10538275</v>
@@ -2115,8 +2038,8 @@
       <c r="H7" s="15">
         <v>725</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>173</v>
+      <c r="I7" s="21">
+        <v>1.2</v>
       </c>
       <c r="J7" s="13">
         <f>0.054*(0.845*G7)</f>
@@ -2128,25 +2051,26 @@
       <c r="L7" s="5">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="E8" s="22">
+        <v>29.5</v>
+      </c>
+      <c r="F8" s="17">
+        <v>7.43</v>
       </c>
       <c r="G8" s="3">
         <v>5659715</v>
@@ -2154,8 +2078,8 @@
       <c r="H8" s="15">
         <v>2389</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>169</v>
+      <c r="I8" s="19">
+        <v>1.6</v>
       </c>
       <c r="J8" s="13">
         <f>0.055*(0.845*G8)</f>
@@ -2167,25 +2091,26 @@
       <c r="L8" s="5">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F9" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="D9" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E9" s="22">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="F9" s="17">
+        <v>9.6300000000000008</v>
       </c>
       <c r="G9" s="3">
         <v>1313271</v>
@@ -2193,8 +2118,8 @@
       <c r="H9" s="2">
         <v>832</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>174</v>
+      <c r="I9" s="19">
+        <v>1.4</v>
       </c>
       <c r="J9" s="13">
         <f>0.067*(0.845*G9)</f>
@@ -2206,25 +2131,26 @@
       <c r="L9" s="5">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="D10" s="23">
+        <v>6.5</v>
+      </c>
+      <c r="E10" s="22">
+        <v>27.6</v>
+      </c>
+      <c r="F10" s="17">
+        <v>6.4</v>
       </c>
       <c r="G10" s="3">
         <v>5471753</v>
@@ -2232,8 +2158,8 @@
       <c r="H10" s="2">
         <v>2479</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>175</v>
+      <c r="I10" s="19">
+        <v>1.3</v>
       </c>
       <c r="J10" s="13">
         <f>0.07*(0.845*G10)</f>
@@ -2245,25 +2171,26 @@
       <c r="L10" s="5">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D11" s="9">
         <v>13</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>43</v>
+      <c r="E11" s="22">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F11" s="17">
+        <v>21.89</v>
       </c>
       <c r="G11" s="3">
         <v>66352469</v>
@@ -2271,8 +2198,8 @@
       <c r="H11" s="2">
         <v>2183</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>176</v>
+      <c r="I11" s="19">
+        <v>0.6</v>
       </c>
       <c r="J11" s="13">
         <f>0.088*(0.845*G11)</f>
@@ -2284,25 +2211,26 @@
       <c r="L11" s="5">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D12" s="9">
         <v>10</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
+      <c r="E12" s="22">
+        <v>30.1</v>
+      </c>
+      <c r="F12" s="17">
+        <v>10.23</v>
       </c>
       <c r="G12" s="3">
         <v>81174000</v>
@@ -2310,8 +2238,8 @@
       <c r="H12" s="2">
         <v>2155</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>177</v>
+      <c r="I12" s="21">
+        <v>2.8</v>
       </c>
       <c r="J12" s="13">
         <f>0.047*(0.845*G12)</f>
@@ -2323,25 +2251,26 @@
       <c r="L12" s="5">
         <v>79</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="D13" s="23">
+        <v>15.5</v>
+      </c>
+      <c r="E13" s="22">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="F13" s="17">
+        <v>31.33</v>
       </c>
       <c r="G13" s="3">
         <v>10812467</v>
@@ -2349,8 +2278,8 @@
       <c r="H13" s="11">
         <v>1262</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>172</v>
+      <c r="I13" s="19">
+        <v>1</v>
       </c>
       <c r="J13" s="13">
         <f>0.248*(0.845*G13)</f>
@@ -2363,24 +2292,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="D14" s="9">
         <v>8</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
+      <c r="E14" s="22">
+        <v>28.9</v>
+      </c>
+      <c r="F14" s="17">
+        <v>26.73</v>
       </c>
       <c r="G14" s="3">
         <v>9849000</v>
@@ -2388,8 +2317,8 @@
       <c r="H14" s="11">
         <v>532</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>174</v>
+      <c r="I14" s="19">
+        <v>1.4</v>
       </c>
       <c r="J14" s="13">
         <f>0.067*(0.845*G14)</f>
@@ -2401,16 +2330,17 @@
       <c r="L14" s="5">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="D15" s="9">
         <v>6</v>
@@ -2418,8 +2348,8 @@
       <c r="E15" s="8">
         <v>27</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>47</v>
+      <c r="F15" s="17">
+        <v>8.5</v>
       </c>
       <c r="G15" s="3">
         <v>329100</v>
@@ -2427,8 +2357,8 @@
       <c r="H15" s="11">
         <v>2334</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>169</v>
+      <c r="I15" s="20">
+        <v>1.6</v>
       </c>
       <c r="J15" s="13">
         <f>0.039*(0.845*G15)</f>
@@ -2440,25 +2370,26 @@
       <c r="L15" s="5">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="D16" s="9">
         <v>13</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>46</v>
+      <c r="E16" s="22">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F16" s="17">
+        <v>10.87</v>
       </c>
       <c r="G16" s="3">
         <v>4625885</v>
@@ -2466,8 +2397,8 @@
       <c r="H16" s="11">
         <v>2186</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>171</v>
+      <c r="I16" s="21">
+        <v>0.7</v>
       </c>
       <c r="J16" s="13">
         <f>0.1*(0.845*G16)</f>
@@ -2479,25 +2410,26 @@
       <c r="L16" s="5">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D17" s="23">
+        <v>14.5</v>
+      </c>
+      <c r="E17" s="22">
+        <v>34.5</v>
+      </c>
+      <c r="F17" s="17">
+        <v>23.75</v>
       </c>
       <c r="G17" s="3">
         <v>60795612</v>
@@ -2505,8 +2437,8 @@
       <c r="H17" s="11">
         <v>2030</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>176</v>
+      <c r="I17" s="19">
+        <v>0.6</v>
       </c>
       <c r="J17" s="13">
         <f>0.16*(0.845*G17)</f>
@@ -2518,16 +2450,17 @@
       <c r="L17" s="5">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D18" s="9">
         <v>16</v>
@@ -2535,8 +2468,8 @@
       <c r="E18" s="8">
         <v>36</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>52</v>
+      <c r="F18" s="17">
+        <v>21.1</v>
       </c>
       <c r="G18" s="3">
         <v>1986096</v>
@@ -2544,8 +2477,8 @@
       <c r="H18" s="2">
         <v>379</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>178</v>
+      <c r="I18" s="19">
+        <v>0.4</v>
       </c>
       <c r="J18" s="13">
         <f>0.1*(0.845*G18)</f>
@@ -2557,25 +2490,26 @@
       <c r="L18" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
+      </c>
+      <c r="D19" s="23">
+        <v>11.5</v>
+      </c>
+      <c r="E19" s="22">
+        <v>31.8</v>
+      </c>
+      <c r="F19" s="17">
+        <v>7.02</v>
       </c>
       <c r="G19" s="3">
         <v>37369</v>
@@ -2583,8 +2517,8 @@
       <c r="H19" s="11">
         <v>5314</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>173</v>
+      <c r="I19" s="20">
+        <v>1.2</v>
       </c>
       <c r="J19" s="13">
         <f>0.023*(0.845*G19)</f>
@@ -2596,25 +2530,26 @@
       <c r="L19" s="5">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="D20" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E20" s="22">
+        <v>32.6</v>
+      </c>
+      <c r="F20" s="17">
+        <v>19.2</v>
       </c>
       <c r="G20" s="3">
         <v>2921262</v>
@@ -2622,8 +2557,8 @@
       <c r="H20" s="11">
         <v>496</v>
       </c>
-      <c r="I20" s="12" t="s">
-        <v>179</v>
+      <c r="I20" s="19">
+        <v>0.9</v>
       </c>
       <c r="J20" s="13">
         <f>0.099*(0.845*G20)</f>
@@ -2635,25 +2570,26 @@
       <c r="L20" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D21" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E21" s="22">
+        <v>32.4</v>
+      </c>
+      <c r="F21" s="17">
+        <v>6.7</v>
       </c>
       <c r="G21" s="3">
         <v>562958</v>
@@ -2661,8 +2597,8 @@
       <c r="H21" s="15">
         <v>3187</v>
       </c>
-      <c r="I21" s="12" t="s">
-        <v>172</v>
+      <c r="I21" s="19">
+        <v>1</v>
       </c>
       <c r="J21" s="13">
         <f>0.05*(0.845*G21)</f>
@@ -2674,16 +2610,17 @@
       <c r="L21" s="5">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="D22" s="9">
         <v>7</v>
@@ -2691,8 +2628,8 @@
       <c r="E22" s="8">
         <v>28</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>54</v>
+      <c r="F22" s="17">
+        <v>23.84</v>
       </c>
       <c r="G22" s="3">
         <v>429344</v>
@@ -2700,8 +2637,8 @@
       <c r="H22" s="11">
         <v>1006</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>180</v>
+      <c r="I22" s="19">
+        <v>3.1</v>
       </c>
       <c r="J22" s="13">
         <f>0.048*(0.845*G22)</f>
@@ -2713,25 +2650,26 @@
       <c r="L22" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="3" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
+      </c>
+      <c r="D23" s="23">
+        <v>10.5</v>
+      </c>
+      <c r="E23" s="22">
+        <v>30.6</v>
+      </c>
+      <c r="F23" s="17">
+        <v>34.78</v>
       </c>
       <c r="G23" s="3">
         <v>622099</v>
@@ -2739,8 +2677,8 @@
       <c r="H23" s="5">
         <v>726</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>181</v>
+      <c r="I23" s="20">
+        <v>0.8</v>
       </c>
       <c r="J23" s="13">
         <f>0.145*(0.845*G23)</f>
@@ -2752,16 +2690,17 @@
       <c r="L23" s="5">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D24" s="9">
         <v>7</v>
@@ -2769,8 +2708,8 @@
       <c r="E24" s="8">
         <v>28</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>55</v>
+      <c r="F24" s="17">
+        <v>6.46</v>
       </c>
       <c r="G24" s="3">
         <v>16900726</v>
@@ -2778,8 +2717,8 @@
       <c r="H24" s="15">
         <v>2158</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>174</v>
+      <c r="I24" s="19">
+        <v>1.4</v>
       </c>
       <c r="J24" s="13">
         <f>0.065*(0.845*G24)</f>
@@ -2791,25 +2730,26 @@
       <c r="L24" s="5">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
+      </c>
+      <c r="D25" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="E25" s="22">
+        <v>25.5</v>
+      </c>
+      <c r="F25" s="17">
+        <v>6.52</v>
       </c>
       <c r="G25" s="3">
         <v>5165802</v>
@@ -2817,8 +2757,8 @@
       <c r="H25" s="5">
         <v>3850</v>
       </c>
-      <c r="I25" s="12" t="s">
-        <v>182</v>
+      <c r="I25" s="19">
+        <v>2.6</v>
       </c>
       <c r="J25" s="13">
         <f>0.028*(0.845*G25)</f>
@@ -2830,25 +2770,26 @@
       <c r="L25" s="5">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="D26" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E26" s="22">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="F26" s="17">
+        <v>11.03</v>
       </c>
       <c r="G26" s="3">
         <v>38005614</v>
@@ -2856,8 +2797,8 @@
       <c r="H26" s="5">
         <v>634</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>183</v>
+      <c r="I26" s="19">
+        <v>0.5</v>
       </c>
       <c r="J26" s="13">
         <f>0.077*(0.845*G26)</f>
@@ -2869,25 +2810,26 @@
       <c r="L26" s="5">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="N26"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="D27" s="9">
         <v>16</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>56</v>
+      <c r="E27" s="22">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F27" s="17">
+        <v>17.73</v>
       </c>
       <c r="G27" s="3">
         <v>10374822</v>
@@ -2895,8 +2837,8 @@
       <c r="H27" s="12">
         <v>1056</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>176</v>
+      <c r="I27" s="19">
+        <v>0.6</v>
       </c>
       <c r="J27" s="13">
         <f>0.125*(0.845*G27)</f>
@@ -2908,25 +2850,26 @@
       <c r="L27" s="5">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="N27"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="D28" s="9">
         <v>6</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>57</v>
+      <c r="E28" s="22">
+        <v>27.2</v>
+      </c>
+      <c r="F28" s="17">
+        <v>23.48</v>
       </c>
       <c r="G28" s="3">
         <v>19861408</v>
@@ -2934,8 +2877,8 @@
       <c r="H28" s="12">
         <v>345</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>179</v>
+      <c r="I28" s="19">
+        <v>0.9</v>
       </c>
       <c r="J28" s="13">
         <f>0.055*(0.845*G28)</f>
@@ -2947,16 +2890,17 @@
       <c r="L28" s="5">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="N28"/>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="D29" s="9">
         <v>10</v>
@@ -2964,7 +2908,7 @@
       <c r="E29" s="8">
         <v>30</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="18">
         <v>25.05</v>
       </c>
       <c r="G29" s="3">
@@ -2973,8 +2917,8 @@
       <c r="H29" s="5">
         <v>377</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>181</v>
+      <c r="I29" s="20">
+        <v>0.8</v>
       </c>
       <c r="J29" s="13">
         <f>0.2*(0.845*G29)</f>
@@ -2986,25 +2930,26 @@
       <c r="L29" s="12">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="N29" s="16"/>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="D30" s="23">
+        <v>5.5</v>
+      </c>
+      <c r="E30" s="22">
+        <v>26.5</v>
+      </c>
+      <c r="F30" s="17">
+        <v>11.39</v>
       </c>
       <c r="G30" s="3">
         <v>5421349</v>
@@ -3012,8 +2957,8 @@
       <c r="H30" s="12">
         <v>664</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>179</v>
+      <c r="I30" s="19">
+        <v>0.9</v>
       </c>
       <c r="J30" s="13">
         <f>0.118*(0.845*G30)</f>
@@ -3025,25 +2970,26 @@
       <c r="L30" s="5">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="D31" s="9">
         <v>5</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>59</v>
+      <c r="E31" s="22">
+        <v>24.9</v>
+      </c>
+      <c r="F31" s="17">
+        <v>20.38</v>
       </c>
       <c r="G31" s="3">
         <v>2062874</v>
@@ -3051,8 +2997,8 @@
       <c r="H31" s="12">
         <v>1023</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>175</v>
+      <c r="I31" s="19">
+        <v>1.3</v>
       </c>
       <c r="J31" s="13">
         <f>0.089*(0.845*G31)</f>
@@ -3064,16 +3010,17 @@
       <c r="L31" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="N31"/>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D32" s="9">
         <v>16</v>
@@ -3081,8 +3028,8 @@
       <c r="E32" s="8">
         <v>36</v>
       </c>
-      <c r="F32" s="2">
-        <v>6.4</v>
+      <c r="F32" s="17">
+        <v>20.63</v>
       </c>
       <c r="G32" s="3">
         <v>46439864</v>
@@ -3090,8 +3037,8 @@
       <c r="H32" s="5">
         <v>1702</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>176</v>
+      <c r="I32" s="21">
+        <v>0.6</v>
       </c>
       <c r="J32" s="13">
         <f>0.223*(0.845*G32)</f>
@@ -3103,25 +3050,26 @@
       <c r="L32" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32"/>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="D33" s="9">
         <v>6</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>58</v>
+      <c r="E33" s="22">
+        <v>27.2</v>
+      </c>
+      <c r="F33" s="17">
+        <v>8.98</v>
       </c>
       <c r="G33" s="3">
         <v>9747355</v>
@@ -3129,8 +3077,8 @@
       <c r="H33" s="5">
         <v>2825</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>184</v>
+      <c r="I33" s="19">
+        <v>1.8</v>
       </c>
       <c r="J33" s="13">
         <f>0.057*(0.845*G33)</f>
@@ -3142,25 +3090,26 @@
       <c r="L33" s="5">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>35</v>
+        <v>66</v>
+      </c>
+      <c r="D34" s="23">
+        <v>11.5</v>
+      </c>
+      <c r="E34" s="22">
+        <v>31.8</v>
+      </c>
+      <c r="F34" s="17">
+        <v>10.47</v>
       </c>
       <c r="G34" s="3">
         <v>8236573</v>
@@ -3168,8 +3117,8 @@
       <c r="H34" s="5">
         <v>2930</v>
       </c>
-      <c r="I34" s="12" t="s">
-        <v>173</v>
+      <c r="I34" s="19">
+        <v>1.2</v>
       </c>
       <c r="J34" s="13">
         <f>0.034*(0.845*G34)</f>
@@ -3181,16 +3130,17 @@
       <c r="L34" s="5">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="D35" s="9">
         <v>20</v>
@@ -3198,7 +3148,7 @@
       <c r="E35" s="8">
         <v>40</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="17">
         <v>45.87</v>
       </c>
       <c r="G35" s="3">
@@ -3207,8 +3157,8 @@
       <c r="H35" s="12">
         <v>510</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>181</v>
+      <c r="I35" s="20">
+        <v>0.8</v>
       </c>
       <c r="J35" s="13">
         <f>0.083*(0.845*G35)</f>
@@ -3220,16 +3170,17 @@
       <c r="L35" s="5">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35"/>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="D36" s="9">
         <v>10</v>
@@ -3237,8 +3188,8 @@
       <c r="E36" s="8">
         <v>30.2</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>61</v>
+      <c r="F36" s="17">
+        <v>19.93</v>
       </c>
       <c r="G36" s="3">
         <v>64767115</v>
@@ -3246,8 +3197,8 @@
       <c r="H36" s="12">
         <v>2233</v>
       </c>
-      <c r="I36" s="12" t="s">
-        <v>185</v>
+      <c r="I36" s="19">
+        <v>2.2999999999999998</v>
       </c>
       <c r="J36" s="13">
         <f>0.044*(0.845*G36)</f>
@@ -3259,40 +3210,111 @@
       <c r="L36" s="5">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N36"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="N37"/>
+      <c r="O37"/>
+    </row>
+    <row r="39" spans="1:15">
       <c r="M39" s="14"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N39"/>
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="N40"/>
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="1:15">
       <c r="M41" s="14"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="43" spans="1:15">
+      <c r="N43"/>
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="1:15">
       <c r="M44" s="14"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44"/>
+      <c r="O44"/>
+    </row>
+    <row r="45" spans="1:15">
       <c r="M45" s="14"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N45"/>
+      <c r="O45"/>
+    </row>
+    <row r="47" spans="1:15">
       <c r="M47" s="14"/>
-    </row>
-    <row r="49" spans="13:13">
+      <c r="N47"/>
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="N48"/>
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="13:15">
       <c r="M49" s="14"/>
-    </row>
-    <row r="50" spans="13:13">
+      <c r="N49"/>
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="13:15">
       <c r="M50" s="14"/>
-    </row>
-    <row r="53" spans="13:13">
+      <c r="N50"/>
+      <c r="O50"/>
+    </row>
+    <row r="53" spans="13:15">
       <c r="M53" s="14"/>
-    </row>
-    <row r="54" spans="13:13">
+      <c r="N53"/>
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="13:15">
       <c r="M54" s="14"/>
     </row>
-    <row r="56" spans="13:13">
+    <row r="55" spans="13:15">
+      <c r="N55"/>
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="13:15">
       <c r="M56" s="14"/>
     </row>
+    <row r="58" spans="13:15">
+      <c r="N58"/>
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="13:15">
+      <c r="N59"/>
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="13:15">
+      <c r="N60"/>
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="13:15">
+      <c r="N61"/>
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="13:15">
+      <c r="N62"/>
+      <c r="O62"/>
+    </row>
+    <row r="64" spans="13:15">
+      <c r="N64"/>
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="14:15">
+      <c r="N65"/>
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="14:15">
+      <c r="N66"/>
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="14:15">
+      <c r="N67"/>
+      <c r="O67"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:K36">
-    <sortCondition ref="C2:C36"/>
+  <sortState ref="N1:Q95">
+    <sortCondition ref="N1:N95"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add legenda score ++ update unemployment rates in percent
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t>AT</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>corruption</t>
+  </si>
+  <si>
+    <t>absoluut-werkloosheid</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,7 +488,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="449">
+  <cellStyleXfs count="451">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -936,8 +938,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -970,8 +974,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="449">
+  <cellStyles count="451">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1196,6 +1201,7 @@
     <cellStyle name="Gevolgde hyperlink" xfId="444" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="446" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="450" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1420,6 +1426,7 @@
     <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1749,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1766,13 +1773,14 @@
     <col min="7" max="7" width="18.125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.625" style="1"/>
+    <col min="10" max="10" width="8.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -1803,185 +1811,204 @@
       <c r="J1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1"/>
+      <c r="N1" s="14"/>
       <c r="O1"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="23">
-        <v>10.5</v>
+        <v>36</v>
+      </c>
+      <c r="D2" s="9">
+        <v>14</v>
       </c>
       <c r="E2" s="22">
-        <v>30.8</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F2" s="17">
-        <v>10.01</v>
+        <v>31.42</v>
       </c>
       <c r="G2" s="3">
-        <v>8584926</v>
+        <v>7202198</v>
       </c>
       <c r="H2" s="2">
-        <v>2165</v>
+        <v>324</v>
       </c>
       <c r="I2" s="21">
-        <v>1.6</v>
-      </c>
-      <c r="J2" s="13">
-        <f>0.049*(0.845*G2)</f>
-        <v>355458.86103000003</v>
-      </c>
-      <c r="K2" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J2" s="24">
+        <f>K2/G2*100</f>
+        <v>14.365</v>
+      </c>
+      <c r="K2" s="13">
+        <f>0.17*(0.845*G2)</f>
+        <v>1034595.7427000001</v>
+      </c>
+      <c r="L2" s="5">
+        <v>89</v>
+      </c>
+      <c r="M2" s="5">
+        <v>43</v>
+      </c>
+      <c r="O2"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="5">
-        <v>72</v>
-      </c>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="23">
-        <v>7.5</v>
+      <c r="D3" s="9">
+        <v>6</v>
       </c>
       <c r="E3" s="22">
-        <v>28.4</v>
+        <v>27.2</v>
       </c>
       <c r="F3" s="17">
-        <v>12.8</v>
+        <v>23.48</v>
       </c>
       <c r="G3" s="3">
-        <v>11258434</v>
-      </c>
-      <c r="H3" s="15">
-        <v>2092</v>
-      </c>
-      <c r="I3" s="21">
-        <v>2.4</v>
-      </c>
-      <c r="J3" s="13">
-        <f>0.073*(0.845*G3)</f>
-        <v>694476.50129000004</v>
-      </c>
-      <c r="K3" s="5">
+        <v>19861408</v>
+      </c>
+      <c r="H3" s="12">
+        <v>345</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="J3" s="24">
+        <f>K3/G3*100</f>
+        <v>4.6475</v>
+      </c>
+      <c r="K3" s="13">
+        <f>0.055*(0.845*G3)</f>
+        <v>923058.93679999991</v>
+      </c>
+      <c r="L3" s="5">
         <v>78</v>
       </c>
-      <c r="L3" s="5">
-        <v>76</v>
-      </c>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="M3" s="5">
+        <v>43</v>
+      </c>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="9">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8">
+        <v>30</v>
+      </c>
+      <c r="F4" s="18">
+        <v>25.05</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7000000</v>
+      </c>
+      <c r="H4" s="5">
+        <v>377</v>
+      </c>
+      <c r="I4" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="J4" s="24">
+        <f>K4/G4*100</f>
+        <v>16.900000000000002</v>
+      </c>
+      <c r="K4" s="13">
+        <f>0.2*(0.845*G4)</f>
+        <v>1183000</v>
+      </c>
+      <c r="L4" s="5">
+        <v>50</v>
+      </c>
+      <c r="M4" s="12">
+        <v>41</v>
+      </c>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="9">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8">
         <v>36</v>
       </c>
-      <c r="D4" s="9">
-        <v>14</v>
-      </c>
-      <c r="E4" s="22">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="F4" s="17">
-        <v>31.42</v>
-      </c>
-      <c r="G4" s="3">
-        <v>7202198</v>
-      </c>
-      <c r="H4" s="2">
-        <v>324</v>
-      </c>
-      <c r="I4" s="21">
-        <v>0.7</v>
-      </c>
-      <c r="J4" s="13">
-        <f>0.17*(0.845*G4)</f>
-        <v>1034595.7427000001</v>
-      </c>
-      <c r="K4" s="5">
-        <v>89</v>
-      </c>
-      <c r="L4" s="5">
-        <v>43</v>
-      </c>
-      <c r="N4"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="9">
-        <v>14</v>
-      </c>
-      <c r="E5" s="22">
-        <v>34.200000000000003</v>
-      </c>
       <c r="F5" s="17">
-        <v>26.82</v>
+        <v>21.1</v>
       </c>
       <c r="G5" s="3">
-        <v>4225316</v>
-      </c>
-      <c r="H5" s="11">
-        <v>755</v>
+        <v>1986096</v>
+      </c>
+      <c r="H5" s="2">
+        <v>379</v>
       </c>
       <c r="I5" s="19">
-        <v>1</v>
-      </c>
-      <c r="J5" s="13">
-        <f>0.146*(0.845*G5)</f>
-        <v>521277.23491999996</v>
-      </c>
-      <c r="K5" s="5">
-        <v>61</v>
+        <v>0.4</v>
+      </c>
+      <c r="J5" s="24">
+        <f>K5/G5*100</f>
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="K5" s="13">
+        <f>0.1*(0.845*G5)</f>
+        <v>167825.11199999999</v>
       </c>
       <c r="L5" s="5">
-        <v>48</v>
-      </c>
-      <c r="N5"/>
-    </row>
-    <row r="6" spans="1:15">
+        <v>34</v>
+      </c>
+      <c r="M5" s="5">
+        <v>55</v>
+      </c>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="23">
         <v>12.5</v>
@@ -1990,1331 +2017,1455 @@
         <v>32.6</v>
       </c>
       <c r="F6" s="17">
-        <v>29.54</v>
+        <v>19.2</v>
       </c>
       <c r="G6" s="3">
-        <v>847008</v>
-      </c>
-      <c r="H6" s="5">
-        <v>2223</v>
+        <v>2921262</v>
+      </c>
+      <c r="H6" s="11">
+        <v>496</v>
       </c>
       <c r="I6" s="19">
-        <v>1.2</v>
-      </c>
-      <c r="J6" s="13">
-        <f>0.14*(0.845*G6)</f>
-        <v>100201.04640000001</v>
-      </c>
-      <c r="K6" s="5">
-        <v>50</v>
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="24">
+        <f>K6/G6*100</f>
+        <v>8.3655000000000008</v>
+      </c>
+      <c r="K6" s="13">
+        <f>0.099*(0.845*G6)</f>
+        <v>244378.17261000004</v>
       </c>
       <c r="L6" s="5">
-        <v>63</v>
-      </c>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="1:15">
+        <v>43</v>
+      </c>
+      <c r="M6" s="5">
+        <v>58</v>
+      </c>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="23">
-        <v>5.5</v>
-      </c>
-      <c r="E7" s="22">
-        <v>26.4</v>
+        <v>69</v>
+      </c>
+      <c r="D7" s="9">
+        <v>20</v>
+      </c>
+      <c r="E7" s="8">
+        <v>40</v>
       </c>
       <c r="F7" s="17">
-        <v>10.07</v>
+        <v>45.87</v>
       </c>
       <c r="G7" s="3">
-        <v>10538275</v>
-      </c>
-      <c r="H7" s="15">
-        <v>725</v>
-      </c>
-      <c r="I7" s="21">
-        <v>1.2</v>
-      </c>
-      <c r="J7" s="13">
-        <f>0.054*(0.845*G7)</f>
-        <v>480861.48824999999</v>
-      </c>
-      <c r="K7" s="5">
-        <v>48</v>
+        <v>77695904</v>
+      </c>
+      <c r="H7" s="12">
+        <v>510</v>
+      </c>
+      <c r="I7" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="24">
+        <f>K7/G7*100</f>
+        <v>7.0135000000000005</v>
+      </c>
+      <c r="K7" s="13">
+        <f>0.083*(0.845*G7)</f>
+        <v>5449202.2270400003</v>
       </c>
       <c r="L7" s="5">
+        <v>26</v>
+      </c>
+      <c r="M7" s="5">
+        <v>45</v>
+      </c>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N7"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="23">
-        <v>8.5</v>
+      <c r="D8" s="9">
+        <v>8</v>
       </c>
       <c r="E8" s="22">
-        <v>29.5</v>
+        <v>28.9</v>
       </c>
       <c r="F8" s="17">
-        <v>7.43</v>
+        <v>26.73</v>
       </c>
       <c r="G8" s="3">
-        <v>5659715</v>
-      </c>
-      <c r="H8" s="15">
-        <v>2389</v>
+        <v>9849000</v>
+      </c>
+      <c r="H8" s="11">
+        <v>532</v>
       </c>
       <c r="I8" s="19">
-        <v>1.6</v>
-      </c>
-      <c r="J8" s="13">
-        <f>0.055*(0.845*G8)</f>
-        <v>263035.254625</v>
-      </c>
-      <c r="K8" s="5">
-        <v>50</v>
+        <v>1.4</v>
+      </c>
+      <c r="J8" s="24">
+        <f>K8/G8*100</f>
+        <v>5.6615000000000002</v>
+      </c>
+      <c r="K8" s="13">
+        <f>0.067*(0.845*G8)</f>
+        <v>557601.13500000001</v>
       </c>
       <c r="L8" s="5">
-        <v>92</v>
-      </c>
-      <c r="N8"/>
-    </row>
-    <row r="9" spans="1:15">
+        <v>83</v>
+      </c>
+      <c r="M8" s="5">
+        <v>54</v>
+      </c>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D9" s="23">
         <v>12.5</v>
       </c>
       <c r="E9" s="22">
-        <v>32.700000000000003</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F9" s="17">
-        <v>9.6300000000000008</v>
+        <v>11.03</v>
       </c>
       <c r="G9" s="3">
-        <v>1313271</v>
-      </c>
-      <c r="H9" s="2">
-        <v>832</v>
+        <v>38005614</v>
+      </c>
+      <c r="H9" s="5">
+        <v>634</v>
       </c>
       <c r="I9" s="19">
-        <v>1.4</v>
-      </c>
-      <c r="J9" s="13">
-        <f>0.067*(0.845*G9)</f>
-        <v>74350.837664999999</v>
-      </c>
-      <c r="K9" s="5">
-        <v>32</v>
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="24">
+        <f>K9/G9*100</f>
+        <v>6.5065</v>
+      </c>
+      <c r="K9" s="13">
+        <f>0.077*(0.845*G9)</f>
+        <v>2472835.2749099997</v>
       </c>
       <c r="L9" s="5">
-        <v>69</v>
-      </c>
-      <c r="N9"/>
-    </row>
-    <row r="10" spans="1:15">
+        <v>52</v>
+      </c>
+      <c r="M9" s="5">
+        <v>61</v>
+      </c>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="23">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="E10" s="22">
-        <v>27.6</v>
+        <v>26.5</v>
       </c>
       <c r="F10" s="17">
-        <v>6.4</v>
+        <v>11.39</v>
       </c>
       <c r="G10" s="3">
-        <v>5471753</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2479</v>
+        <v>5421349</v>
+      </c>
+      <c r="H10" s="12">
+        <v>664</v>
       </c>
       <c r="I10" s="19">
-        <v>1.3</v>
-      </c>
-      <c r="J10" s="13">
-        <f>0.07*(0.845*G10)</f>
-        <v>323654.18995000003</v>
-      </c>
-      <c r="K10" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="J10" s="24">
+        <f>K10/G10*100</f>
+        <v>9.9710000000000001</v>
+      </c>
+      <c r="K10" s="13">
+        <f>0.118*(0.845*G10)</f>
+        <v>540562.70878999995</v>
+      </c>
+      <c r="L10" s="5">
+        <v>72</v>
+      </c>
+      <c r="M10" s="5">
+        <v>50</v>
+      </c>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L10" s="5">
-        <v>89</v>
-      </c>
-      <c r="N10"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="9">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="D11" s="23">
+        <v>5.5</v>
       </c>
       <c r="E11" s="22">
-        <v>33.299999999999997</v>
+        <v>26.4</v>
       </c>
       <c r="F11" s="17">
-        <v>21.89</v>
+        <v>10.07</v>
       </c>
       <c r="G11" s="3">
-        <v>66352469</v>
-      </c>
-      <c r="H11" s="2">
-        <v>2183</v>
-      </c>
-      <c r="I11" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="J11" s="13">
-        <f>0.088*(0.845*G11)</f>
-        <v>4933969.5948399995</v>
-      </c>
-      <c r="K11" s="5">
-        <v>77</v>
+        <v>10538275</v>
+      </c>
+      <c r="H11" s="15">
+        <v>725</v>
+      </c>
+      <c r="I11" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="J11" s="24">
+        <f>K11/G11*100</f>
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="K11" s="13">
+        <f>0.054*(0.845*G11)</f>
+        <v>480861.48824999999</v>
       </c>
       <c r="L11" s="5">
-        <v>69</v>
-      </c>
-      <c r="N11"/>
-    </row>
-    <row r="12" spans="1:15">
+        <v>48</v>
+      </c>
+      <c r="M11" s="5">
+        <v>51</v>
+      </c>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>78</v>
+        <v>106</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="9">
-        <v>10</v>
+        <v>67</v>
+      </c>
+      <c r="D12" s="23">
+        <v>10.5</v>
       </c>
       <c r="E12" s="22">
-        <v>30.1</v>
+        <v>30.6</v>
       </c>
       <c r="F12" s="17">
-        <v>10.23</v>
+        <v>34.78</v>
       </c>
       <c r="G12" s="3">
-        <v>81174000</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2155</v>
-      </c>
-      <c r="I12" s="21">
-        <v>2.8</v>
-      </c>
-      <c r="J12" s="13">
-        <f>0.047*(0.845*G12)</f>
-        <v>3223825.41</v>
-      </c>
-      <c r="K12" s="5">
-        <v>58</v>
+        <v>622099</v>
+      </c>
+      <c r="H12" s="5">
+        <v>726</v>
+      </c>
+      <c r="I12" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="24">
+        <f>K12/G12*100</f>
+        <v>12.252499999999998</v>
+      </c>
+      <c r="K12" s="13">
+        <f>0.145*(0.845*G12)</f>
+        <v>76222.679974999992</v>
       </c>
       <c r="L12" s="5">
-        <v>79</v>
-      </c>
-      <c r="N12"/>
-    </row>
-    <row r="13" spans="1:15">
+        <v>50</v>
+      </c>
+      <c r="M12" s="5">
+        <v>42</v>
+      </c>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="23">
-        <v>15.5</v>
+        <v>45</v>
+      </c>
+      <c r="D13" s="9">
+        <v>14</v>
       </c>
       <c r="E13" s="22">
-        <v>35.700000000000003</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F13" s="17">
-        <v>31.33</v>
+        <v>26.82</v>
       </c>
       <c r="G13" s="3">
-        <v>10812467</v>
+        <v>4225316</v>
       </c>
       <c r="H13" s="11">
-        <v>1262</v>
+        <v>755</v>
       </c>
       <c r="I13" s="19">
         <v>1</v>
       </c>
-      <c r="J13" s="13">
-        <f>0.248*(0.845*G13)</f>
-        <v>2265860.58452</v>
-      </c>
-      <c r="K13" s="5">
-        <v>60</v>
+      <c r="J13" s="24">
+        <f>K13/G13*100</f>
+        <v>12.337</v>
+      </c>
+      <c r="K13" s="13">
+        <f>0.146*(0.845*G13)</f>
+        <v>521277.23491999996</v>
       </c>
       <c r="L13" s="5">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>61</v>
+      </c>
+      <c r="M13" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="9">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="D14" s="23">
+        <v>12.5</v>
       </c>
       <c r="E14" s="22">
-        <v>28.9</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="F14" s="17">
-        <v>26.73</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="G14" s="3">
-        <v>9849000</v>
-      </c>
-      <c r="H14" s="11">
-        <v>532</v>
+        <v>1313271</v>
+      </c>
+      <c r="H14" s="2">
+        <v>832</v>
       </c>
       <c r="I14" s="19">
         <v>1.4</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="24">
+        <f>K14/G14*100</f>
+        <v>5.6615000000000002</v>
+      </c>
+      <c r="K14" s="13">
         <f>0.067*(0.845*G14)</f>
-        <v>557601.13500000001</v>
-      </c>
-      <c r="K14" s="5">
-        <v>83</v>
+        <v>74350.837664999999</v>
       </c>
       <c r="L14" s="5">
-        <v>54</v>
-      </c>
-      <c r="N14"/>
-    </row>
-    <row r="15" spans="1:15">
+        <v>32</v>
+      </c>
+      <c r="M14" s="5">
+        <v>69</v>
+      </c>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>101</v>
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D15" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" s="8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" s="17">
-        <v>8.5</v>
+        <v>23.84</v>
       </c>
       <c r="G15" s="3">
-        <v>329100</v>
+        <v>429344</v>
       </c>
       <c r="H15" s="11">
-        <v>2334</v>
-      </c>
-      <c r="I15" s="20">
-        <v>1.6</v>
-      </c>
-      <c r="J15" s="13">
-        <f>0.039*(0.845*G15)</f>
-        <v>10845.4905</v>
-      </c>
-      <c r="K15" s="5">
+        <v>1006</v>
+      </c>
+      <c r="I15" s="19">
+        <v>3.1</v>
+      </c>
+      <c r="J15" s="24">
+        <f>K15/G15*100</f>
+        <v>4.0560000000000009</v>
+      </c>
+      <c r="K15" s="13">
+        <f>0.048*(0.845*G15)</f>
+        <v>17414.192640000001</v>
+      </c>
+      <c r="L15" s="5">
+        <v>51</v>
+      </c>
+      <c r="M15" s="5">
+        <v>55</v>
+      </c>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="9">
         <v>5</v>
       </c>
-      <c r="L15" s="5">
-        <v>79</v>
-      </c>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="9">
-        <v>13</v>
-      </c>
       <c r="E16" s="22">
-        <v>33.299999999999997</v>
+        <v>24.9</v>
       </c>
       <c r="F16" s="17">
-        <v>10.87</v>
+        <v>20.38</v>
       </c>
       <c r="G16" s="3">
-        <v>4625885</v>
-      </c>
-      <c r="H16" s="11">
-        <v>2186</v>
-      </c>
-      <c r="I16" s="21">
-        <v>0.7</v>
-      </c>
-      <c r="J16" s="13">
-        <f>0.1*(0.845*G16)</f>
-        <v>390887.28249999997</v>
-      </c>
-      <c r="K16" s="5">
-        <v>66</v>
+        <v>2062874</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1023</v>
+      </c>
+      <c r="I16" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="J16" s="24">
+        <f>K16/G16*100</f>
+        <v>7.5204999999999993</v>
+      </c>
+      <c r="K16" s="13">
+        <f>0.089*(0.845*G16)</f>
+        <v>155138.43917</v>
       </c>
       <c r="L16" s="5">
-        <v>74</v>
-      </c>
-      <c r="N16"/>
-    </row>
-    <row r="17" spans="1:14">
+        <v>67</v>
+      </c>
+      <c r="M16" s="5">
+        <v>58</v>
+      </c>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="23">
-        <v>14.5</v>
-      </c>
       <c r="E17" s="22">
-        <v>34.5</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="F17" s="17">
-        <v>23.75</v>
+        <v>17.73</v>
       </c>
       <c r="G17" s="3">
-        <v>60795612</v>
-      </c>
-      <c r="H17" s="11">
-        <v>2030</v>
+        <v>10374822</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1056</v>
       </c>
       <c r="I17" s="19">
         <v>0.6</v>
       </c>
-      <c r="J17" s="13">
-        <f>0.16*(0.845*G17)</f>
+      <c r="J17" s="24">
+        <f>K17/G17*100</f>
+        <v>10.5625</v>
+      </c>
+      <c r="K17" s="13">
+        <f>0.125*(0.845*G17)</f>
+        <v>1095840.57375</v>
+      </c>
+      <c r="L17" s="5">
+        <v>88</v>
+      </c>
+      <c r="M17" s="5">
+        <v>63</v>
+      </c>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="23">
+        <v>15.5</v>
+      </c>
+      <c r="E18" s="22">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="F18" s="17">
+        <v>31.33</v>
+      </c>
+      <c r="G18" s="3">
+        <v>10812467</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1262</v>
+      </c>
+      <c r="I18" s="19">
+        <v>1</v>
+      </c>
+      <c r="J18" s="24">
+        <f>K18/G18*100</f>
+        <v>20.956</v>
+      </c>
+      <c r="K18" s="13">
+        <f>0.248*(0.845*G18)</f>
+        <v>2265860.58452</v>
+      </c>
+      <c r="L18" s="5">
+        <v>60</v>
+      </c>
+      <c r="M18" s="5">
+        <v>43</v>
+      </c>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="9">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8">
+        <v>36</v>
+      </c>
+      <c r="F19" s="17">
+        <v>20.63</v>
+      </c>
+      <c r="G19" s="3">
+        <v>46439864</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1702</v>
+      </c>
+      <c r="I19" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="J19" s="24">
+        <f>K19/G19*100</f>
+        <v>18.843499999999995</v>
+      </c>
+      <c r="K19" s="13">
+        <f>0.223*(0.845*G19)</f>
+        <v>8750895.7728399988</v>
+      </c>
+      <c r="L19" s="5">
+        <v>49</v>
+      </c>
+      <c r="M19" s="5">
+        <v>60</v>
+      </c>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="23">
+        <v>14.5</v>
+      </c>
+      <c r="E20" s="22">
+        <v>34.5</v>
+      </c>
+      <c r="F20" s="17">
+        <v>23.75</v>
+      </c>
+      <c r="G20" s="3">
+        <v>60795612</v>
+      </c>
+      <c r="H20" s="11">
+        <v>2030</v>
+      </c>
+      <c r="I20" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="J20" s="24">
+        <f>K20/G20*100</f>
+        <v>13.52</v>
+      </c>
+      <c r="K20" s="13">
+        <f>0.16*(0.845*G20)</f>
         <v>8219566.7423999999</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L20" s="5">
         <v>61</v>
       </c>
-      <c r="L17" s="5">
+      <c r="M20" s="5">
         <v>43</v>
       </c>
-      <c r="N17"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="9">
-        <v>16</v>
-      </c>
-      <c r="E18" s="8">
-        <v>36</v>
-      </c>
-      <c r="F18" s="17">
-        <v>21.1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1986096</v>
-      </c>
-      <c r="H18" s="2">
-        <v>379</v>
-      </c>
-      <c r="I18" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="J18" s="13">
-        <f>0.1*(0.845*G18)</f>
-        <v>167825.11199999999</v>
-      </c>
-      <c r="K18" s="5">
-        <v>34</v>
-      </c>
-      <c r="L18" s="5">
-        <v>55</v>
-      </c>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="23">
-        <v>11.5</v>
-      </c>
-      <c r="E19" s="22">
-        <v>31.8</v>
-      </c>
-      <c r="F19" s="17">
-        <v>7.02</v>
-      </c>
-      <c r="G19" s="3">
-        <v>37369</v>
-      </c>
-      <c r="H19" s="11">
-        <v>5314</v>
-      </c>
-      <c r="I19" s="20">
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="E21" s="22">
+        <v>28.4</v>
+      </c>
+      <c r="F21" s="17">
+        <v>12.8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>11258434</v>
+      </c>
+      <c r="H21" s="15">
+        <v>2092</v>
+      </c>
+      <c r="I21" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="J21" s="24">
+        <f>K21/G21*100</f>
+        <v>6.1685000000000008</v>
+      </c>
+      <c r="K21" s="13">
+        <f>0.073*(0.845*G21)</f>
+        <v>694476.50129000004</v>
+      </c>
+      <c r="L21" s="5">
+        <v>78</v>
+      </c>
+      <c r="M21" s="5">
+        <v>76</v>
+      </c>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="9">
+        <v>10</v>
+      </c>
+      <c r="E22" s="22">
+        <v>30.1</v>
+      </c>
+      <c r="F22" s="17">
+        <v>10.23</v>
+      </c>
+      <c r="G22" s="3">
+        <v>81174000</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2155</v>
+      </c>
+      <c r="I22" s="21">
+        <v>2.8</v>
+      </c>
+      <c r="J22" s="24">
+        <f>K22/G22*100</f>
+        <v>3.9714999999999998</v>
+      </c>
+      <c r="K22" s="13">
+        <f>0.047*(0.845*G22)</f>
+        <v>3223825.41</v>
+      </c>
+      <c r="L22" s="5">
+        <v>58</v>
+      </c>
+      <c r="M22" s="5">
+        <v>79</v>
+      </c>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="9">
+        <v>7</v>
+      </c>
+      <c r="E23" s="8">
+        <v>28</v>
+      </c>
+      <c r="F23" s="17">
+        <v>6.46</v>
+      </c>
+      <c r="G23" s="3">
+        <v>16900726</v>
+      </c>
+      <c r="H23" s="15">
+        <v>2158</v>
+      </c>
+      <c r="I23" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="J23" s="24">
+        <f>K23/G23*100</f>
+        <v>5.4924999999999997</v>
+      </c>
+      <c r="K23" s="13">
+        <f>0.065*(0.845*G23)</f>
+        <v>928272.37555</v>
+      </c>
+      <c r="L23" s="5">
+        <v>73</v>
+      </c>
+      <c r="M23" s="5">
+        <v>83</v>
+      </c>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="23">
+        <v>10.5</v>
+      </c>
+      <c r="E24" s="22">
+        <v>30.8</v>
+      </c>
+      <c r="F24" s="17">
+        <v>10.01</v>
+      </c>
+      <c r="G24" s="3">
+        <v>8584926</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2165</v>
+      </c>
+      <c r="I24" s="21">
+        <v>1.6</v>
+      </c>
+      <c r="J24" s="24">
+        <f>K24/G24*100</f>
+        <v>4.1405000000000003</v>
+      </c>
+      <c r="K24" s="13">
+        <f>0.049*(0.845*G24)</f>
+        <v>355458.86103000003</v>
+      </c>
+      <c r="L24" s="5">
+        <v>57</v>
+      </c>
+      <c r="M24" s="5">
+        <v>72</v>
+      </c>
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="9">
+        <v>13</v>
+      </c>
+      <c r="E25" s="22">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F25" s="17">
+        <v>21.89</v>
+      </c>
+      <c r="G25" s="3">
+        <v>66352469</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2183</v>
+      </c>
+      <c r="I25" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="J25" s="24">
+        <f>K25/G25*100</f>
+        <v>7.4359999999999999</v>
+      </c>
+      <c r="K25" s="13">
+        <f>0.088*(0.845*G25)</f>
+        <v>4933969.5948399995</v>
+      </c>
+      <c r="L25" s="5">
+        <v>77</v>
+      </c>
+      <c r="M25" s="5">
+        <v>69</v>
+      </c>
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="9">
+        <v>13</v>
+      </c>
+      <c r="E26" s="22">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F26" s="17">
+        <v>10.87</v>
+      </c>
+      <c r="G26" s="3">
+        <v>4625885</v>
+      </c>
+      <c r="H26" s="11">
+        <v>2186</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0.7</v>
+      </c>
+      <c r="J26" s="24">
+        <f>K26/G26*100</f>
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="K26" s="13">
+        <f>0.1*(0.845*G26)</f>
+        <v>390887.28249999997</v>
+      </c>
+      <c r="L26" s="5">
+        <v>66</v>
+      </c>
+      <c r="M26" s="5">
+        <v>74</v>
+      </c>
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E27" s="22">
+        <v>32.6</v>
+      </c>
+      <c r="F27" s="17">
+        <v>29.54</v>
+      </c>
+      <c r="G27" s="3">
+        <v>847008</v>
+      </c>
+      <c r="H27" s="5">
+        <v>2223</v>
+      </c>
+      <c r="I27" s="19">
         <v>1.2</v>
       </c>
-      <c r="J19" s="13">
-        <f>0.023*(0.845*G19)</f>
-        <v>726.26651500000003</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="J27" s="24">
+        <f>K27/G27*100</f>
+        <v>11.83</v>
+      </c>
+      <c r="K27" s="13">
+        <f>0.14*(0.845*G27)</f>
+        <v>100201.04640000001</v>
+      </c>
+      <c r="L27" s="5">
+        <v>50</v>
+      </c>
+      <c r="M27" s="5">
+        <v>63</v>
+      </c>
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="5">
-        <v>86</v>
-      </c>
-      <c r="N19"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="23">
-        <v>12.5</v>
-      </c>
-      <c r="E20" s="22">
-        <v>32.6</v>
-      </c>
-      <c r="F20" s="17">
-        <v>19.2</v>
-      </c>
-      <c r="G20" s="3">
-        <v>2921262</v>
-      </c>
-      <c r="H20" s="11">
-        <v>496</v>
-      </c>
-      <c r="I20" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="J20" s="13">
-        <f>0.099*(0.845*G20)</f>
-        <v>244378.17261000004</v>
-      </c>
-      <c r="K20" s="5">
-        <v>43</v>
-      </c>
-      <c r="L20" s="5">
-        <v>58</v>
-      </c>
-      <c r="N20"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="23">
-        <v>12.5</v>
-      </c>
-      <c r="E21" s="22">
-        <v>32.4</v>
-      </c>
-      <c r="F21" s="17">
-        <v>6.7</v>
-      </c>
-      <c r="G21" s="3">
-        <v>562958</v>
-      </c>
-      <c r="H21" s="15">
-        <v>3187</v>
-      </c>
-      <c r="I21" s="19">
-        <v>1</v>
-      </c>
-      <c r="J21" s="13">
-        <f>0.05*(0.845*G21)</f>
-        <v>23784.9755</v>
-      </c>
-      <c r="K21" s="5">
-        <v>49</v>
-      </c>
-      <c r="L21" s="5">
-        <v>82</v>
-      </c>
-      <c r="N21"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="9">
+      <c r="B28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="9">
+        <v>10</v>
+      </c>
+      <c r="E28" s="8">
+        <v>30.2</v>
+      </c>
+      <c r="F28" s="17">
+        <v>19.93</v>
+      </c>
+      <c r="G28" s="3">
+        <v>64767115</v>
+      </c>
+      <c r="H28" s="12">
+        <v>2233</v>
+      </c>
+      <c r="I28" s="19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J28" s="24">
+        <f>K28/G28*100</f>
+        <v>3.718</v>
+      </c>
+      <c r="K28" s="13">
+        <f>0.044*(0.845*G28)</f>
+        <v>2408041.3356999997</v>
+      </c>
+      <c r="L28" s="5">
+        <v>85</v>
+      </c>
+      <c r="M28" s="5">
+        <v>78</v>
+      </c>
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="9">
+        <v>6</v>
+      </c>
+      <c r="E29" s="8">
+        <v>27</v>
+      </c>
+      <c r="F29" s="17">
+        <v>8.5</v>
+      </c>
+      <c r="G29" s="3">
+        <v>329100</v>
+      </c>
+      <c r="H29" s="11">
+        <v>2334</v>
+      </c>
+      <c r="I29" s="20">
+        <v>1.6</v>
+      </c>
+      <c r="J29" s="24">
+        <f>K29/G29*100</f>
+        <v>3.2954999999999997</v>
+      </c>
+      <c r="K29" s="13">
+        <f>0.039*(0.845*G29)</f>
+        <v>10845.4905</v>
+      </c>
+      <c r="L29" s="5">
+        <v>5</v>
+      </c>
+      <c r="M29" s="5">
+        <v>79</v>
+      </c>
+      <c r="O29" s="16"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="8">
-        <v>28</v>
-      </c>
-      <c r="F22" s="17">
-        <v>23.84</v>
-      </c>
-      <c r="G22" s="3">
-        <v>429344</v>
-      </c>
-      <c r="H22" s="11">
-        <v>1006</v>
-      </c>
-      <c r="I22" s="19">
-        <v>3.1</v>
-      </c>
-      <c r="J22" s="13">
-        <f>0.048*(0.845*G22)</f>
-        <v>17414.192640000001</v>
-      </c>
-      <c r="K22" s="5">
-        <v>51</v>
-      </c>
-      <c r="L22" s="5">
-        <v>55</v>
-      </c>
-      <c r="N22"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="23">
-        <v>10.5</v>
-      </c>
-      <c r="E23" s="22">
-        <v>30.6</v>
-      </c>
-      <c r="F23" s="17">
-        <v>34.78</v>
-      </c>
-      <c r="G23" s="3">
-        <v>622099</v>
-      </c>
-      <c r="H23" s="5">
-        <v>726</v>
-      </c>
-      <c r="I23" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="J23" s="13">
-        <f>0.145*(0.845*G23)</f>
-        <v>76222.679974999992</v>
-      </c>
-      <c r="K23" s="5">
-        <v>50</v>
-      </c>
-      <c r="L23" s="5">
-        <v>42</v>
-      </c>
-      <c r="N23"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="9">
-        <v>7</v>
-      </c>
-      <c r="E24" s="8">
-        <v>28</v>
-      </c>
-      <c r="F24" s="17">
-        <v>6.46</v>
-      </c>
-      <c r="G24" s="3">
-        <v>16900726</v>
-      </c>
-      <c r="H24" s="15">
-        <v>2158</v>
-      </c>
-      <c r="I24" s="19">
-        <v>1.4</v>
-      </c>
-      <c r="J24" s="13">
-        <f>0.065*(0.845*G24)</f>
-        <v>928272.37555</v>
-      </c>
-      <c r="K24" s="5">
-        <v>73</v>
-      </c>
-      <c r="L24" s="5">
-        <v>83</v>
-      </c>
-      <c r="N24"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="E25" s="22">
-        <v>25.5</v>
-      </c>
-      <c r="F25" s="17">
-        <v>6.52</v>
-      </c>
-      <c r="G25" s="3">
-        <v>5165802</v>
-      </c>
-      <c r="H25" s="5">
-        <v>3850</v>
-      </c>
-      <c r="I25" s="19">
-        <v>2.6</v>
-      </c>
-      <c r="J25" s="13">
-        <f>0.028*(0.845*G25)</f>
-        <v>122222.87531999999</v>
-      </c>
-      <c r="K25" s="5">
-        <v>59</v>
-      </c>
-      <c r="L25" s="5">
-        <v>86</v>
-      </c>
-      <c r="N25"/>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="23">
-        <v>12.5</v>
-      </c>
-      <c r="E26" s="22">
-        <v>32.799999999999997</v>
-      </c>
-      <c r="F26" s="17">
-        <v>11.03</v>
-      </c>
-      <c r="G26" s="3">
-        <v>38005614</v>
-      </c>
-      <c r="H26" s="5">
-        <v>634</v>
-      </c>
-      <c r="I26" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="J26" s="13">
-        <f>0.077*(0.845*G26)</f>
-        <v>2472835.2749099997</v>
-      </c>
-      <c r="K26" s="5">
-        <v>52</v>
-      </c>
-      <c r="L26" s="5">
-        <v>61</v>
-      </c>
-      <c r="N26"/>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="9">
-        <v>16</v>
-      </c>
-      <c r="E27" s="22">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="F27" s="17">
-        <v>17.73</v>
-      </c>
-      <c r="G27" s="3">
-        <v>10374822</v>
-      </c>
-      <c r="H27" s="12">
-        <v>1056</v>
-      </c>
-      <c r="I27" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="J27" s="13">
-        <f>0.125*(0.845*G27)</f>
-        <v>1095840.57375</v>
-      </c>
-      <c r="K27" s="5">
-        <v>88</v>
-      </c>
-      <c r="L27" s="5">
-        <v>63</v>
-      </c>
-      <c r="N27"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="9">
-        <v>6</v>
-      </c>
-      <c r="E28" s="22">
-        <v>27.2</v>
-      </c>
-      <c r="F28" s="17">
-        <v>23.48</v>
-      </c>
-      <c r="G28" s="3">
-        <v>19861408</v>
-      </c>
-      <c r="H28" s="12">
-        <v>345</v>
-      </c>
-      <c r="I28" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="J28" s="13">
-        <f>0.055*(0.845*G28)</f>
-        <v>923058.93679999991</v>
-      </c>
-      <c r="K28" s="5">
-        <v>78</v>
-      </c>
-      <c r="L28" s="5">
-        <v>43</v>
-      </c>
-      <c r="N28"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="9">
-        <v>10</v>
-      </c>
-      <c r="E29" s="8">
-        <v>30</v>
-      </c>
-      <c r="F29" s="18">
-        <v>25.05</v>
-      </c>
-      <c r="G29" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="H29" s="5">
-        <v>377</v>
-      </c>
-      <c r="I29" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="J29" s="13">
-        <f>0.2*(0.845*G29)</f>
-        <v>1183000</v>
-      </c>
-      <c r="K29" s="5">
-        <v>50</v>
-      </c>
-      <c r="L29" s="12">
-        <v>41</v>
-      </c>
-      <c r="N29" s="16"/>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="B30" s="3" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D30" s="23">
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
       <c r="E30" s="22">
-        <v>26.5</v>
+        <v>29.5</v>
       </c>
       <c r="F30" s="17">
-        <v>11.39</v>
+        <v>7.43</v>
       </c>
       <c r="G30" s="3">
-        <v>5421349</v>
-      </c>
-      <c r="H30" s="12">
-        <v>664</v>
+        <v>5659715</v>
+      </c>
+      <c r="H30" s="15">
+        <v>2389</v>
       </c>
       <c r="I30" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="J30" s="13">
-        <f>0.118*(0.845*G30)</f>
-        <v>540562.70878999995</v>
-      </c>
-      <c r="K30" s="5">
-        <v>72</v>
+        <v>1.6</v>
+      </c>
+      <c r="J30" s="24">
+        <f>K30/G30*100</f>
+        <v>4.6475</v>
+      </c>
+      <c r="K30" s="13">
+        <f>0.055*(0.845*G30)</f>
+        <v>263035.254625</v>
       </c>
       <c r="L30" s="5">
         <v>50</v>
       </c>
-      <c r="N30"/>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="M30" s="5">
+        <v>92</v>
+      </c>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="9">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="D31" s="23">
+        <v>6.5</v>
       </c>
       <c r="E31" s="22">
-        <v>24.9</v>
+        <v>27.6</v>
       </c>
       <c r="F31" s="17">
-        <v>20.38</v>
+        <v>6.4</v>
       </c>
       <c r="G31" s="3">
-        <v>2062874</v>
-      </c>
-      <c r="H31" s="12">
-        <v>1023</v>
+        <v>5471753</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2479</v>
       </c>
       <c r="I31" s="19">
         <v>1.3</v>
       </c>
-      <c r="J31" s="13">
-        <f>0.089*(0.845*G31)</f>
-        <v>155138.43917</v>
-      </c>
-      <c r="K31" s="5">
-        <v>67</v>
+      <c r="J31" s="24">
+        <f>K31/G31*100</f>
+        <v>5.9150000000000009</v>
+      </c>
+      <c r="K31" s="13">
+        <f>0.07*(0.845*G31)</f>
+        <v>323654.18995000003</v>
       </c>
       <c r="L31" s="5">
-        <v>58</v>
-      </c>
-      <c r="N31"/>
-    </row>
-    <row r="32" spans="1:14">
+        <v>77</v>
+      </c>
+      <c r="M31" s="5">
+        <v>89</v>
+      </c>
+      <c r="O31"/>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D32" s="9">
-        <v>16</v>
-      </c>
-      <c r="E32" s="8">
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="E32" s="22">
+        <v>27.2</v>
       </c>
       <c r="F32" s="17">
-        <v>20.63</v>
+        <v>8.98</v>
       </c>
       <c r="G32" s="3">
-        <v>46439864</v>
+        <v>9747355</v>
       </c>
       <c r="H32" s="5">
-        <v>1702</v>
-      </c>
-      <c r="I32" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="J32" s="13">
-        <f>0.223*(0.845*G32)</f>
-        <v>8750895.7728399988</v>
-      </c>
-      <c r="K32" s="5">
+        <v>2825</v>
+      </c>
+      <c r="I32" s="19">
+        <v>1.8</v>
+      </c>
+      <c r="J32" s="24">
+        <f>K32/G32*100</f>
+        <v>4.8164999999999996</v>
+      </c>
+      <c r="K32" s="13">
+        <f>0.057*(0.845*G32)</f>
+        <v>469481.35357500002</v>
+      </c>
+      <c r="L32" s="5">
+        <v>85</v>
+      </c>
+      <c r="M32" s="5">
+        <v>87</v>
+      </c>
+      <c r="O32"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="23">
+        <v>11.5</v>
+      </c>
+      <c r="E33" s="22">
+        <v>31.8</v>
+      </c>
+      <c r="F33" s="17">
+        <v>10.47</v>
+      </c>
+      <c r="G33" s="3">
+        <v>8236573</v>
+      </c>
+      <c r="H33" s="5">
+        <v>2930</v>
+      </c>
+      <c r="I33" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="J33" s="24">
+        <f>K33/G33*100</f>
+        <v>2.8729999999999998</v>
+      </c>
+      <c r="K33" s="13">
+        <f>0.034*(0.845*G33)</f>
+        <v>236636.74228999999</v>
+      </c>
+      <c r="L33" s="5">
+        <v>31</v>
+      </c>
+      <c r="M33" s="5">
+        <v>86</v>
+      </c>
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E34" s="22">
+        <v>32.4</v>
+      </c>
+      <c r="F34" s="17">
+        <v>6.7</v>
+      </c>
+      <c r="G34" s="3">
+        <v>562958</v>
+      </c>
+      <c r="H34" s="15">
+        <v>3187</v>
+      </c>
+      <c r="I34" s="19">
+        <v>1</v>
+      </c>
+      <c r="J34" s="24">
+        <f>K34/G34*100</f>
+        <v>4.2250000000000005</v>
+      </c>
+      <c r="K34" s="13">
+        <f>0.05*(0.845*G34)</f>
+        <v>23784.9755</v>
+      </c>
+      <c r="L34" s="5">
         <v>49</v>
       </c>
-      <c r="L32" s="5">
-        <v>60</v>
-      </c>
-      <c r="N32"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="9">
-        <v>6</v>
-      </c>
-      <c r="E33" s="22">
-        <v>27.2</v>
-      </c>
-      <c r="F33" s="17">
-        <v>8.98</v>
-      </c>
-      <c r="G33" s="3">
-        <v>9747355</v>
-      </c>
-      <c r="H33" s="5">
-        <v>2825</v>
-      </c>
-      <c r="I33" s="19">
-        <v>1.8</v>
-      </c>
-      <c r="J33" s="13">
-        <f>0.057*(0.845*G33)</f>
-        <v>469481.35357500002</v>
-      </c>
-      <c r="K33" s="5">
-        <v>85</v>
-      </c>
-      <c r="L33" s="5">
-        <v>87</v>
-      </c>
-      <c r="N33"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="23">
+      <c r="M34" s="5">
+        <v>82</v>
+      </c>
+      <c r="O34"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="E35" s="22">
+        <v>25.5</v>
+      </c>
+      <c r="F35" s="17">
+        <v>6.52</v>
+      </c>
+      <c r="G35" s="3">
+        <v>5165802</v>
+      </c>
+      <c r="H35" s="5">
+        <v>3850</v>
+      </c>
+      <c r="I35" s="19">
+        <v>2.6</v>
+      </c>
+      <c r="J35" s="24">
+        <f>K35/G35*100</f>
+        <v>2.3659999999999997</v>
+      </c>
+      <c r="K35" s="13">
+        <f>0.028*(0.845*G35)</f>
+        <v>122222.87531999999</v>
+      </c>
+      <c r="L35" s="5">
+        <v>59</v>
+      </c>
+      <c r="M35" s="5">
+        <v>86</v>
+      </c>
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="23">
         <v>11.5</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E36" s="22">
         <v>31.8</v>
       </c>
-      <c r="F34" s="17">
-        <v>10.47</v>
-      </c>
-      <c r="G34" s="3">
-        <v>8236573</v>
-      </c>
-      <c r="H34" s="5">
-        <v>2930</v>
-      </c>
-      <c r="I34" s="19">
+      <c r="F36" s="17">
+        <v>7.02</v>
+      </c>
+      <c r="G36" s="3">
+        <v>37369</v>
+      </c>
+      <c r="H36" s="11">
+        <v>5314</v>
+      </c>
+      <c r="I36" s="20">
         <v>1.2</v>
       </c>
-      <c r="J34" s="13">
-        <f>0.034*(0.845*G34)</f>
-        <v>236636.74228999999</v>
-      </c>
-      <c r="K34" s="5">
+      <c r="J36" s="24">
+        <f>K36/G36*100</f>
+        <v>1.9435</v>
+      </c>
+      <c r="K36" s="13">
+        <f>0.023*(0.845*G36)</f>
+        <v>726.26651500000003</v>
+      </c>
+      <c r="L36" s="5">
         <v>31</v>
       </c>
-      <c r="L34" s="5">
+      <c r="M36" s="5">
         <v>86</v>
       </c>
-      <c r="N34"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="9">
-        <v>20</v>
-      </c>
-      <c r="E35" s="8">
-        <v>40</v>
-      </c>
-      <c r="F35" s="17">
-        <v>45.87</v>
-      </c>
-      <c r="G35" s="3">
-        <v>77695904</v>
-      </c>
-      <c r="H35" s="12">
-        <v>510</v>
-      </c>
-      <c r="I35" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="J35" s="13">
-        <f>0.083*(0.845*G35)</f>
-        <v>5449202.2270400003</v>
-      </c>
-      <c r="K35" s="5">
-        <v>26</v>
-      </c>
-      <c r="L35" s="5">
-        <v>45</v>
-      </c>
-      <c r="N35"/>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="9">
-        <v>10</v>
-      </c>
-      <c r="E36" s="8">
-        <v>30.2</v>
-      </c>
-      <c r="F36" s="17">
-        <v>19.93</v>
-      </c>
-      <c r="G36" s="3">
-        <v>64767115</v>
-      </c>
-      <c r="H36" s="12">
-        <v>2233</v>
-      </c>
-      <c r="I36" s="19">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J36" s="13">
-        <f>0.044*(0.845*G36)</f>
-        <v>2408041.3356999997</v>
-      </c>
-      <c r="K36" s="5">
-        <v>85</v>
-      </c>
-      <c r="L36" s="5">
-        <v>78</v>
-      </c>
-      <c r="N36"/>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="N37"/>
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="1:16">
       <c r="O37"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="M39" s="14"/>
-      <c r="N39"/>
+      <c r="P37"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="N39" s="14"/>
       <c r="O39"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="N40"/>
+      <c r="P39"/>
+    </row>
+    <row r="40" spans="1:16">
       <c r="O40"/>
-    </row>
-    <row r="41" spans="1:15">
-      <c r="M41" s="14"/>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="N43"/>
+      <c r="P40"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="N41" s="14"/>
+    </row>
+    <row r="43" spans="1:16">
       <c r="O43"/>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="M44" s="14"/>
-      <c r="N44"/>
+      <c r="P43"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="N44" s="14"/>
       <c r="O44"/>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="M45" s="14"/>
-      <c r="N45"/>
+      <c r="P44"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="N45" s="14"/>
       <c r="O45"/>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="M47" s="14"/>
-      <c r="N47"/>
+      <c r="P45"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="N47" s="14"/>
       <c r="O47"/>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="N48"/>
+      <c r="P47"/>
+    </row>
+    <row r="48" spans="1:16">
       <c r="O48"/>
-    </row>
-    <row r="49" spans="13:15">
-      <c r="M49" s="14"/>
-      <c r="N49"/>
+      <c r="P48"/>
+    </row>
+    <row r="49" spans="14:16">
+      <c r="N49" s="14"/>
       <c r="O49"/>
-    </row>
-    <row r="50" spans="13:15">
-      <c r="M50" s="14"/>
-      <c r="N50"/>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="14:16">
+      <c r="N50" s="14"/>
       <c r="O50"/>
-    </row>
-    <row r="53" spans="13:15">
-      <c r="M53" s="14"/>
-      <c r="N53"/>
+      <c r="P50"/>
+    </row>
+    <row r="53" spans="14:16">
+      <c r="N53" s="14"/>
       <c r="O53"/>
-    </row>
-    <row r="54" spans="13:15">
-      <c r="M54" s="14"/>
-    </row>
-    <row r="55" spans="13:15">
-      <c r="N55"/>
+      <c r="P53"/>
+    </row>
+    <row r="54" spans="14:16">
+      <c r="N54" s="14"/>
+    </row>
+    <row r="55" spans="14:16">
       <c r="O55"/>
-    </row>
-    <row r="56" spans="13:15">
-      <c r="M56" s="14"/>
-    </row>
-    <row r="58" spans="13:15">
-      <c r="N58"/>
+      <c r="P55"/>
+    </row>
+    <row r="56" spans="14:16">
+      <c r="N56" s="14"/>
+    </row>
+    <row r="58" spans="14:16">
       <c r="O58"/>
-    </row>
-    <row r="59" spans="13:15">
-      <c r="N59"/>
+      <c r="P58"/>
+    </row>
+    <row r="59" spans="14:16">
       <c r="O59"/>
-    </row>
-    <row r="60" spans="13:15">
-      <c r="N60"/>
+      <c r="P59"/>
+    </row>
+    <row r="60" spans="14:16">
       <c r="O60"/>
-    </row>
-    <row r="61" spans="13:15">
-      <c r="N61"/>
+      <c r="P60"/>
+    </row>
+    <row r="61" spans="14:16">
       <c r="O61"/>
-    </row>
-    <row r="62" spans="13:15">
-      <c r="N62"/>
+      <c r="P61"/>
+    </row>
+    <row r="62" spans="14:16">
       <c r="O62"/>
-    </row>
-    <row r="64" spans="13:15">
-      <c r="N64"/>
+      <c r="P62"/>
+    </row>
+    <row r="64" spans="14:16">
       <c r="O64"/>
-    </row>
-    <row r="65" spans="14:15">
-      <c r="N65"/>
+      <c r="P64"/>
+    </row>
+    <row r="65" spans="15:16">
       <c r="O65"/>
-    </row>
-    <row r="66" spans="14:15">
-      <c r="N66"/>
+      <c r="P65"/>
+    </row>
+    <row r="66" spans="15:16">
       <c r="O66"/>
-    </row>
-    <row r="67" spans="14:15">
-      <c r="N67"/>
+      <c r="P66"/>
+    </row>
+    <row r="67" spans="15:16">
       <c r="O67"/>
+      <c r="P67"/>
     </row>
   </sheetData>
-  <sortState ref="N1:Q95">
-    <sortCondition ref="N1:N95"/>
+  <sortState ref="A2:M36">
+    <sortCondition ref="H2:H36"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>